<commit_message>
Update met oude projecten
</commit_message>
<xml_diff>
--- a/output/ArtDiver_result.xlsx
+++ b/output/ArtDiver_result.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM39"/>
+  <dimension ref="A1:AM73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -637,27 +637,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HHNK-B14C0141</t>
+          <t>B14C0049</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>105360.042</v>
-      </c>
-      <c r="D2" t="n">
-        <v>530342.04</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="n">
-        <v>0.164</v>
-      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" s="2" t="n">
-        <v>43391.29166666666</v>
-      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
@@ -677,60 +669,42 @@
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="n">
-        <v>0.066</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0.5800000000000001</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr"/>
       <c r="AG2" t="inlineStr"/>
       <c r="AH2" t="inlineStr"/>
       <c r="AI2" t="inlineStr"/>
-      <c r="AJ2" s="2" t="n">
-        <v>43391.29166666666</v>
-      </c>
-      <c r="AK2" s="2" t="n">
-        <v>44180.54861111111</v>
-      </c>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
       <c r="AL2" t="inlineStr">
         <is>
-          <t>HHNK-B14C0141</t>
+          <t>B14C0049</t>
         </is>
       </c>
       <c r="AM2" t="inlineStr">
         <is>
-          <t>HHNK-B14C0141_1</t>
+          <t>B14C0049_2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HHNK-B14C0141</t>
+          <t>B14C0049</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
-        <v>105360.042</v>
-      </c>
-      <c r="D3" t="n">
-        <v>530342.04</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
-        <v>0.164</v>
-      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" s="2" t="n">
-        <v>44180.54861111111</v>
-      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
@@ -750,58 +724,42 @@
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="n">
-        <v>0.066</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>0.5800000000000001</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
       <c r="AF3" t="inlineStr"/>
       <c r="AG3" t="inlineStr"/>
       <c r="AH3" t="inlineStr"/>
       <c r="AI3" t="inlineStr"/>
-      <c r="AJ3" s="2" t="n">
-        <v>44180.54861111111</v>
-      </c>
+      <c r="AJ3" t="inlineStr"/>
       <c r="AK3" t="inlineStr"/>
       <c r="AL3" t="inlineStr">
         <is>
-          <t>HHNK-B14C0141</t>
+          <t>B14C0049</t>
         </is>
       </c>
       <c r="AM3" t="inlineStr">
         <is>
-          <t>HHNK-B14C0141_1</t>
+          <t>B14C0049_3</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>HHNK-B14C0141</t>
+          <t>B14C0054</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="n">
-        <v>105360.042</v>
-      </c>
-      <c r="D4" t="n">
-        <v>530342.04</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="n">
-        <v>0.164</v>
-      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" s="2" t="n">
-        <v>43391.29166666666</v>
-      </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
@@ -821,58 +779,42 @@
       <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr"/>
-      <c r="AC4" t="n">
-        <v>0.094</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>4.920000000000001</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
       <c r="AF4" t="inlineStr"/>
       <c r="AG4" t="inlineStr"/>
       <c r="AH4" t="inlineStr"/>
       <c r="AI4" t="inlineStr"/>
-      <c r="AJ4" s="2" t="n">
-        <v>43391.29166666666</v>
-      </c>
+      <c r="AJ4" t="inlineStr"/>
       <c r="AK4" t="inlineStr"/>
       <c r="AL4" t="inlineStr">
         <is>
-          <t>HHNK-B14C0141</t>
+          <t>B14C0054</t>
         </is>
       </c>
       <c r="AM4" t="inlineStr">
         <is>
-          <t>HHNK-B14C0141_2</t>
+          <t>B14C0054_3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHNK-B14C0146</t>
+          <t>B14C0061</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>106284.9</v>
-      </c>
-      <c r="D5" t="n">
-        <v>529505.249</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="n">
-        <v>-0.207</v>
-      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" s="2" t="n">
-        <v>43404.29166666666</v>
-      </c>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
@@ -892,58 +834,42 @@
       <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr"/>
-      <c r="AC5" t="n">
-        <v>-0.266</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>0.03999999999999998</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
       <c r="AF5" t="inlineStr"/>
       <c r="AG5" t="inlineStr"/>
       <c r="AH5" t="inlineStr"/>
       <c r="AI5" t="inlineStr"/>
-      <c r="AJ5" s="2" t="n">
-        <v>43404.29166666666</v>
-      </c>
+      <c r="AJ5" t="inlineStr"/>
       <c r="AK5" t="inlineStr"/>
       <c r="AL5" t="inlineStr">
         <is>
-          <t>HHNK-B14C0146</t>
+          <t>B14C0061</t>
         </is>
       </c>
       <c r="AM5" t="inlineStr">
         <is>
-          <t>HHNK-B14C0146_1</t>
+          <t>B14C0061_2</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHNK-B14C0146</t>
+          <t>B14C0143</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" t="n">
-        <v>106284.9</v>
-      </c>
-      <c r="D6" t="n">
-        <v>529505.249</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="n">
-        <v>-0.207</v>
-      </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" s="2" t="n">
-        <v>43404.29166666666</v>
-      </c>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
@@ -963,58 +889,42 @@
       <c r="Z6" t="inlineStr"/>
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="n">
-        <v>-0.309</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>4.51</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
       <c r="AF6" t="inlineStr"/>
       <c r="AG6" t="inlineStr"/>
       <c r="AH6" t="inlineStr"/>
       <c r="AI6" t="inlineStr"/>
-      <c r="AJ6" s="2" t="n">
-        <v>43404.29166666666</v>
-      </c>
+      <c r="AJ6" t="inlineStr"/>
       <c r="AK6" t="inlineStr"/>
       <c r="AL6" t="inlineStr">
         <is>
-          <t>HHNK-B14C0146</t>
+          <t>B14C0143</t>
         </is>
       </c>
       <c r="AM6" t="inlineStr">
         <is>
-          <t>HHNK-B14C0146_2</t>
+          <t>B14C0143_1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PB_1_001_04P001442</t>
+          <t>B14C0143</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>104902.088</v>
-      </c>
-      <c r="D7" t="n">
-        <v>528228.1310000001</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="n">
-        <v>-1.044</v>
-      </c>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" s="2" t="n">
-        <v>43388.29166666666</v>
-      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
@@ -1034,60 +944,42 @@
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr"/>
-      <c r="AC7" t="n">
-        <v>0.466</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>2.45</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr"/>
       <c r="AG7" t="inlineStr"/>
       <c r="AH7" t="inlineStr"/>
       <c r="AI7" t="inlineStr"/>
-      <c r="AJ7" s="2" t="n">
-        <v>43388.29166666666</v>
-      </c>
-      <c r="AK7" s="2" t="n">
-        <v>44074.52986111111</v>
-      </c>
+      <c r="AJ7" t="inlineStr"/>
+      <c r="AK7" t="inlineStr"/>
       <c r="AL7" t="inlineStr">
         <is>
-          <t>PB_1_001_04P001442_F-374</t>
+          <t>B14C0143</t>
         </is>
       </c>
       <c r="AM7" t="inlineStr">
         <is>
-          <t>PB_1_001_04P001442_1</t>
+          <t>B14C0143_2</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>PB_1_001_04P001442</t>
+          <t>B14C0144</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>1</v>
       </c>
-      <c r="C8" t="n">
-        <v>104902.088</v>
-      </c>
-      <c r="D8" t="n">
-        <v>528228.1310000001</v>
-      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="n">
-        <v>-1.044</v>
-      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" s="2" t="n">
-        <v>44074.52986111111</v>
-      </c>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
@@ -1107,58 +999,42 @@
       <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr"/>
-      <c r="AC8" t="n">
-        <v>0.466</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>2.45</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="inlineStr"/>
       <c r="AG8" t="inlineStr"/>
       <c r="AH8" t="inlineStr"/>
       <c r="AI8" t="inlineStr"/>
-      <c r="AJ8" s="2" t="n">
-        <v>44074.52986111111</v>
-      </c>
+      <c r="AJ8" t="inlineStr"/>
       <c r="AK8" t="inlineStr"/>
       <c r="AL8" t="inlineStr">
         <is>
-          <t>PB_1_001_04P001442_F-374</t>
+          <t>B14C0144</t>
         </is>
       </c>
       <c r="AM8" t="inlineStr">
         <is>
-          <t>PB_1_001_04P001442_1</t>
+          <t>B14C0144_1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>PB_1_001_04P001442</t>
+          <t>B14C0144</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
-      </c>
-      <c r="C9" t="n">
-        <v>104902.167</v>
-      </c>
-      <c r="D9" t="n">
-        <v>528228.205</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="n">
-        <v>-0.9540000000000001</v>
-      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" s="2" t="n">
-        <v>44074.53958333333</v>
-      </c>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
@@ -1178,58 +1054,42 @@
       <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr"/>
-      <c r="AC9" t="n">
-        <v>0.296</v>
-      </c>
-      <c r="AD9" t="n">
-        <v>21.63</v>
-      </c>
-      <c r="AE9" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
       <c r="AF9" t="inlineStr"/>
       <c r="AG9" t="inlineStr"/>
       <c r="AH9" t="inlineStr"/>
       <c r="AI9" t="inlineStr"/>
-      <c r="AJ9" s="2" t="n">
-        <v>44074.53958333333</v>
-      </c>
+      <c r="AJ9" t="inlineStr"/>
       <c r="AK9" t="inlineStr"/>
       <c r="AL9" t="inlineStr">
         <is>
-          <t>PB_1_001_04P001442_F-2</t>
+          <t>B14C0144</t>
         </is>
       </c>
       <c r="AM9" t="inlineStr">
         <is>
-          <t>PB_1_001_04P001442_3</t>
+          <t>B14C0144_2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>PB_1_001_04P001442</t>
+          <t>B14C0149</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
-      </c>
-      <c r="C10" t="n">
-        <v>104902.167</v>
-      </c>
-      <c r="D10" t="n">
-        <v>528228.205</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="n">
-        <v>-0.9540000000000001</v>
-      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" s="2" t="n">
-        <v>43388.29166666666</v>
-      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -1249,60 +1109,42 @@
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr"/>
-      <c r="AC10" t="n">
-        <v>0.296</v>
-      </c>
-      <c r="AD10" t="n">
-        <v>21.65</v>
-      </c>
-      <c r="AE10" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="inlineStr"/>
       <c r="AG10" t="inlineStr"/>
       <c r="AH10" t="inlineStr"/>
       <c r="AI10" t="inlineStr"/>
-      <c r="AJ10" s="2" t="n">
-        <v>43388.29166666666</v>
-      </c>
-      <c r="AK10" s="2" t="n">
-        <v>44074.53958333333</v>
-      </c>
+      <c r="AJ10" t="inlineStr"/>
+      <c r="AK10" t="inlineStr"/>
       <c r="AL10" t="inlineStr">
         <is>
-          <t>PB_1_001_04P001442_F-2</t>
+          <t>B14C0149</t>
         </is>
       </c>
       <c r="AM10" t="inlineStr">
         <is>
-          <t>PB_1_001_04P001442_3</t>
+          <t>B14C0149_1</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PB_1_002_04P001442</t>
+          <t>B14C0149</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="n">
-        <v>105097.059</v>
-      </c>
-      <c r="D11" t="n">
-        <v>528341.072</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="n">
-        <v>-1.258</v>
-      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" s="2" t="n">
-        <v>43388.29166666666</v>
-      </c>
+      <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
@@ -1322,59 +1164,49 @@
       <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr"/>
-      <c r="AC11" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="AD11" t="n">
-        <v>3.66</v>
-      </c>
-      <c r="AE11" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
       <c r="AF11" t="inlineStr"/>
       <c r="AG11" t="inlineStr"/>
       <c r="AH11" t="inlineStr"/>
       <c r="AI11" t="inlineStr"/>
-      <c r="AJ11" s="2" t="n">
-        <v>43388.29166666666</v>
-      </c>
-      <c r="AK11" s="2" t="n">
-        <v>44074.57569444444</v>
-      </c>
+      <c r="AJ11" t="inlineStr"/>
+      <c r="AK11" t="inlineStr"/>
       <c r="AL11" t="inlineStr">
         <is>
-          <t>PB_1_002_04P001442_F-375</t>
+          <t>B14C0149</t>
         </is>
       </c>
       <c r="AM11" t="inlineStr">
         <is>
-          <t>PB_1_002_04P001442_1</t>
+          <t>B14C0149_2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PB_1_002_04P001442</t>
+          <t>HHNK-B14C0141</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>105097.059</v>
+        <v>105360.042</v>
       </c>
       <c r="D12" t="n">
-        <v>528341.072</v>
+        <v>530342.04</v>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
-        <v>-1.258</v>
+        <v>0.164</v>
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" s="2" t="n">
-        <v>44074.57569444444</v>
+        <v>43391.29166666666</v>
       </c>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
@@ -1396,10 +1228,10 @@
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr"/>
       <c r="AC12" t="n">
-        <v>0.002</v>
+        <v>0.066</v>
       </c>
       <c r="AD12" t="n">
-        <v>3.66</v>
+        <v>0.5800000000000001</v>
       </c>
       <c r="AE12" t="n">
         <v>1</v>
@@ -1409,43 +1241,43 @@
       <c r="AH12" t="inlineStr"/>
       <c r="AI12" t="inlineStr"/>
       <c r="AJ12" s="2" t="n">
-        <v>44074.57569444444</v>
+        <v>43391.29166666666</v>
       </c>
       <c r="AK12" t="inlineStr"/>
       <c r="AL12" t="inlineStr">
         <is>
-          <t>PB_1_002_04P001442_F-375</t>
+          <t>HHNK-B14C0141</t>
         </is>
       </c>
       <c r="AM12" t="inlineStr">
         <is>
-          <t>PB_1_002_04P001442_1</t>
+          <t>HHNK-B14C0141_1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PB_1_002_04P001442</t>
+          <t>HHNK-B14C0141</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>105097.075</v>
+        <v>105360.042</v>
       </c>
       <c r="D13" t="n">
-        <v>528341.068</v>
+        <v>530342.04</v>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
-        <v>-1.178</v>
+        <v>0.164</v>
       </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" s="2" t="n">
-        <v>43388.29166666666</v>
+        <v>43391.29166666666</v>
       </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
@@ -1467,10 +1299,10 @@
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr"/>
       <c r="AC13" t="n">
-        <v>-0.018</v>
+        <v>0.094</v>
       </c>
       <c r="AD13" t="n">
-        <v>24.96</v>
+        <v>4.920000000000001</v>
       </c>
       <c r="AE13" t="n">
         <v>1</v>
@@ -1480,45 +1312,43 @@
       <c r="AH13" t="inlineStr"/>
       <c r="AI13" t="inlineStr"/>
       <c r="AJ13" s="2" t="n">
-        <v>43388.29166666666</v>
-      </c>
-      <c r="AK13" s="2" t="n">
-        <v>44074.59236111111</v>
-      </c>
+        <v>43391.29166666666</v>
+      </c>
+      <c r="AK13" t="inlineStr"/>
       <c r="AL13" t="inlineStr">
         <is>
-          <t>PB_1_002_04P001442_F-2</t>
+          <t>HHNK-B14C0141</t>
         </is>
       </c>
       <c r="AM13" t="inlineStr">
         <is>
-          <t>PB_1_002_04P001442_3</t>
+          <t>HHNK-B14C0141_2</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>PB_1_002_04P001442</t>
+          <t>HHNK-B14C0146</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>105097.075</v>
+        <v>106284.9</v>
       </c>
       <c r="D14" t="n">
-        <v>528341.068</v>
+        <v>529505.249</v>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
-        <v>-1.178</v>
+        <v>-0.207</v>
       </c>
       <c r="H14" t="inlineStr"/>
       <c r="I14" s="2" t="n">
-        <v>44074.59236111111</v>
+        <v>43404.29166666666</v>
       </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
@@ -1540,10 +1370,10 @@
       <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="inlineStr"/>
       <c r="AC14" t="n">
-        <v>-0.018</v>
+        <v>-0.266</v>
       </c>
       <c r="AD14" t="n">
-        <v>25.02</v>
+        <v>0.03999999999999998</v>
       </c>
       <c r="AE14" t="n">
         <v>1</v>
@@ -1553,43 +1383,43 @@
       <c r="AH14" t="inlineStr"/>
       <c r="AI14" t="inlineStr"/>
       <c r="AJ14" s="2" t="n">
-        <v>44074.59236111111</v>
+        <v>43404.29166666666</v>
       </c>
       <c r="AK14" t="inlineStr"/>
       <c r="AL14" t="inlineStr">
         <is>
-          <t>PB_1_002_04P001442_F-2</t>
+          <t>HHNK-B14C0146</t>
         </is>
       </c>
       <c r="AM14" t="inlineStr">
         <is>
-          <t>PB_1_002_04P001442_3</t>
+          <t>HHNK-B14C0146_1</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>PB_1_003_04P001442</t>
+          <t>HHNK-B14C0146</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>105401.868</v>
+        <v>106284.9</v>
       </c>
       <c r="D15" t="n">
-        <v>528165.502</v>
+        <v>529505.249</v>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
-        <v>-0.8009999999999999</v>
+        <v>-0.207</v>
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" s="2" t="n">
-        <v>43389.29166666666</v>
+        <v>43404.29166666666</v>
       </c>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
@@ -1611,10 +1441,10 @@
       <c r="AA15" t="inlineStr"/>
       <c r="AB15" t="inlineStr"/>
       <c r="AC15" t="n">
-        <v>0.119</v>
+        <v>-0.309</v>
       </c>
       <c r="AD15" t="n">
-        <v>3.11</v>
+        <v>4.51</v>
       </c>
       <c r="AE15" t="n">
         <v>1</v>
@@ -1624,44 +1454,36 @@
       <c r="AH15" t="inlineStr"/>
       <c r="AI15" t="inlineStr"/>
       <c r="AJ15" s="2" t="n">
-        <v>43389.29166666666</v>
+        <v>43404.29166666666</v>
       </c>
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="inlineStr">
         <is>
-          <t>PB_1_003_04P001442_F-337</t>
+          <t>HHNK-B14C0146</t>
         </is>
       </c>
       <c r="AM15" t="inlineStr">
         <is>
-          <t>PB_1_003_04P001442_1</t>
+          <t>HHNK-B14C0146_2</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PB_1_003_04P001442</t>
+          <t>PB2_T10108_F-220</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3</v>
-      </c>
-      <c r="C16" t="n">
-        <v>105401.924</v>
-      </c>
-      <c r="D16" t="n">
-        <v>528165.52</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
-      <c r="G16" t="n">
-        <v>-0.74</v>
-      </c>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" s="2" t="n">
-        <v>43388.29166666666</v>
-      </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
@@ -1681,59 +1503,49 @@
       <c r="Z16" t="inlineStr"/>
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr"/>
-      <c r="AC16" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="AD16" t="n">
-        <v>29.61</v>
-      </c>
-      <c r="AE16" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC16" t="inlineStr"/>
+      <c r="AD16" t="inlineStr"/>
+      <c r="AE16" t="inlineStr"/>
       <c r="AF16" t="inlineStr"/>
       <c r="AG16" t="inlineStr"/>
       <c r="AH16" t="inlineStr"/>
       <c r="AI16" t="inlineStr"/>
-      <c r="AJ16" s="2" t="n">
-        <v>43388.29166666666</v>
-      </c>
-      <c r="AK16" s="2" t="n">
-        <v>44075.48125</v>
-      </c>
+      <c r="AJ16" t="inlineStr"/>
+      <c r="AK16" t="inlineStr"/>
       <c r="AL16" t="inlineStr">
         <is>
-          <t>PB_1_003_04P001442_F-2</t>
+          <t>PB2_T10108_F-220</t>
         </is>
       </c>
       <c r="AM16" t="inlineStr">
         <is>
-          <t>PB_1_003_04P001442_3</t>
+          <t>PB2_T10108_F-220_1</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>PB_1_003_04P001442</t>
+          <t>PB_1_001_04P001442</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>105401.924</v>
+        <v>104902.088</v>
       </c>
       <c r="D17" t="n">
-        <v>528165.52</v>
+        <v>528228.1310000001</v>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="n">
-        <v>-0.74</v>
+        <v>-1.044</v>
       </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" s="2" t="n">
-        <v>44075.48125</v>
+        <v>43388.29166666666</v>
       </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
@@ -1755,10 +1567,10 @@
       <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="inlineStr"/>
       <c r="AC17" t="n">
-        <v>-0.1</v>
+        <v>0.466</v>
       </c>
       <c r="AD17" t="n">
-        <v>29.61</v>
+        <v>2.45</v>
       </c>
       <c r="AE17" t="n">
         <v>1</v>
@@ -1768,43 +1580,43 @@
       <c r="AH17" t="inlineStr"/>
       <c r="AI17" t="inlineStr"/>
       <c r="AJ17" s="2" t="n">
-        <v>44075.48125</v>
+        <v>43388.29166666666</v>
       </c>
       <c r="AK17" t="inlineStr"/>
       <c r="AL17" t="inlineStr">
         <is>
-          <t>PB_1_003_04P001442_F-2</t>
+          <t>PB_1_001_04P001442_F-374</t>
         </is>
       </c>
       <c r="AM17" t="inlineStr">
         <is>
-          <t>PB_1_003_04P001442_3</t>
+          <t>PB_1_001_04P001442_1</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PB_1_004_04P001442-01</t>
+          <t>PB_1_001_04P001442</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" t="n">
-        <v>104741.43</v>
+        <v>104902.167</v>
       </c>
       <c r="D18" t="n">
-        <v>528280.213</v>
+        <v>528228.205</v>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="n">
-        <v>10.208</v>
+        <v>-0.9540000000000001</v>
       </c>
       <c r="H18" t="inlineStr"/>
       <c r="I18" s="2" t="n">
-        <v>43389.29166666666</v>
+        <v>43388.29166666666</v>
       </c>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
@@ -1826,10 +1638,10 @@
       <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="inlineStr"/>
       <c r="AC18" t="n">
-        <v>11.338</v>
+        <v>0.296</v>
       </c>
       <c r="AD18" t="n">
-        <v>13.39</v>
+        <v>21.65</v>
       </c>
       <c r="AE18" t="n">
         <v>1</v>
@@ -1839,44 +1651,36 @@
       <c r="AH18" t="inlineStr"/>
       <c r="AI18" t="inlineStr"/>
       <c r="AJ18" s="2" t="n">
-        <v>43389.29166666666</v>
+        <v>43388.29166666666</v>
       </c>
       <c r="AK18" t="inlineStr"/>
       <c r="AL18" t="inlineStr">
         <is>
-          <t>PB_1_004_04P001442-01_F-204</t>
+          <t>PB_1_001_04P001442_F-2</t>
         </is>
       </c>
       <c r="AM18" t="inlineStr">
         <is>
-          <t>PB_1_004_04P001442-01_1</t>
+          <t>PB_1_001_04P001442_3</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>PB_1_004_04P001442-01</t>
+          <t>PB_1_001_04P001442</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>3</v>
-      </c>
-      <c r="C19" t="n">
-        <v>104741.437</v>
-      </c>
-      <c r="D19" t="n">
-        <v>528280.191</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
-      <c r="G19" t="n">
-        <v>10.24</v>
-      </c>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" s="2" t="n">
-        <v>43389.29166666666</v>
-      </c>
+      <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
@@ -1896,57 +1700,49 @@
       <c r="Z19" t="inlineStr"/>
       <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="inlineStr"/>
-      <c r="AC19" t="n">
-        <v>11.34</v>
-      </c>
-      <c r="AD19" t="n">
-        <v>33.3</v>
-      </c>
-      <c r="AE19" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC19" t="inlineStr"/>
+      <c r="AD19" t="inlineStr"/>
+      <c r="AE19" t="inlineStr"/>
       <c r="AF19" t="inlineStr"/>
       <c r="AG19" t="inlineStr"/>
       <c r="AH19" t="inlineStr"/>
       <c r="AI19" t="inlineStr"/>
-      <c r="AJ19" s="2" t="n">
-        <v>43389.29166666666</v>
-      </c>
+      <c r="AJ19" t="inlineStr"/>
       <c r="AK19" t="inlineStr"/>
       <c r="AL19" t="inlineStr">
         <is>
-          <t>PB_1_004_04P001442-01_F-2</t>
+          <t>PB_1_001_04P001442_F-924</t>
         </is>
       </c>
       <c r="AM19" t="inlineStr">
         <is>
-          <t>PB_1_004_04P001442-01_3</t>
+          <t>PB_1_001_04P001442_2</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01</t>
+          <t>PB_1_002_04P001442</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>104701.644</v>
+        <v>105097.059</v>
       </c>
       <c r="D20" t="n">
-        <v>528274.721</v>
+        <v>528341.072</v>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="n">
-        <v>7.84</v>
+        <v>-1.258</v>
       </c>
       <c r="H20" t="inlineStr"/>
       <c r="I20" s="2" t="n">
-        <v>43468.29166666666</v>
+        <v>43388.29166666666</v>
       </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
@@ -1968,10 +1764,10 @@
       <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="inlineStr"/>
       <c r="AC20" t="n">
-        <v>7.35</v>
+        <v>0.002</v>
       </c>
       <c r="AD20" t="n">
-        <v>11</v>
+        <v>3.66</v>
       </c>
       <c r="AE20" t="n">
         <v>1</v>
@@ -1981,45 +1777,43 @@
       <c r="AH20" t="inlineStr"/>
       <c r="AI20" t="inlineStr"/>
       <c r="AJ20" s="2" t="n">
-        <v>43468.29166666666</v>
-      </c>
-      <c r="AK20" s="2" t="n">
-        <v>43501.46666666667</v>
-      </c>
+        <v>43388.29166666666</v>
+      </c>
+      <c r="AK20" t="inlineStr"/>
       <c r="AL20" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01_F-264</t>
+          <t>PB_1_002_04P001442_F-375</t>
         </is>
       </c>
       <c r="AM20" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01_1</t>
+          <t>PB_1_002_04P001442_1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01</t>
+          <t>PB_1_002_04P001442</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C21" t="n">
-        <v>104701.644</v>
+        <v>105097.075</v>
       </c>
       <c r="D21" t="n">
-        <v>528274.721</v>
+        <v>528341.068</v>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
-        <v>7.84</v>
+        <v>-1.178</v>
       </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" s="2" t="n">
-        <v>43501.46666666667</v>
+        <v>43388.29166666666</v>
       </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
@@ -2041,10 +1835,10 @@
       <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="inlineStr"/>
       <c r="AC21" t="n">
-        <v>7.35</v>
+        <v>-0.018</v>
       </c>
       <c r="AD21" t="n">
-        <v>11</v>
+        <v>24.96</v>
       </c>
       <c r="AE21" t="n">
         <v>1</v>
@@ -2054,46 +1848,36 @@
       <c r="AH21" t="inlineStr"/>
       <c r="AI21" t="inlineStr"/>
       <c r="AJ21" s="2" t="n">
-        <v>43501.46666666667</v>
-      </c>
-      <c r="AK21" s="2" t="n">
-        <v>44074.48611111111</v>
-      </c>
+        <v>43388.29166666666</v>
+      </c>
+      <c r="AK21" t="inlineStr"/>
       <c r="AL21" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01_F-264</t>
+          <t>PB_1_002_04P001442_F-2</t>
         </is>
       </c>
       <c r="AM21" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01_1</t>
+          <t>PB_1_002_04P001442_3</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01</t>
+          <t>PB_1_002_04P001442</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" t="n">
-        <v>104701.644</v>
-      </c>
-      <c r="D22" t="n">
-        <v>528274.721</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
-      <c r="G22" t="n">
-        <v>7.84</v>
-      </c>
+      <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
-      <c r="I22" s="2" t="n">
-        <v>44074.48611111111</v>
-      </c>
+      <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
@@ -2113,59 +1897,49 @@
       <c r="Z22" t="inlineStr"/>
       <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="inlineStr"/>
-      <c r="AC22" t="n">
-        <v>9.036</v>
-      </c>
-      <c r="AD22" t="n">
-        <v>12.686</v>
-      </c>
-      <c r="AE22" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC22" t="inlineStr"/>
+      <c r="AD22" t="inlineStr"/>
+      <c r="AE22" t="inlineStr"/>
       <c r="AF22" t="inlineStr"/>
       <c r="AG22" t="inlineStr"/>
       <c r="AH22" t="inlineStr"/>
       <c r="AI22" t="inlineStr"/>
-      <c r="AJ22" s="2" t="n">
-        <v>44074.48611111111</v>
-      </c>
-      <c r="AK22" s="2" t="n">
-        <v>44375.61458333334</v>
-      </c>
+      <c r="AJ22" t="inlineStr"/>
+      <c r="AK22" t="inlineStr"/>
       <c r="AL22" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01_F-264</t>
+          <t>PB_1_002_04P001442_F-975</t>
         </is>
       </c>
       <c r="AM22" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01_1</t>
+          <t>PB_1_002_04P001442_2</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01</t>
+          <t>PB_1_003_04P001442</t>
         </is>
       </c>
       <c r="B23" t="n">
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>104701.644</v>
+        <v>105401.868</v>
       </c>
       <c r="D23" t="n">
-        <v>528274.721</v>
+        <v>528165.502</v>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
-        <v>9.720000000000001</v>
+        <v>-0.8009999999999999</v>
       </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" s="2" t="n">
-        <v>44375.61458333334</v>
+        <v>43389.29166666666</v>
       </c>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
@@ -2187,10 +1961,10 @@
       <c r="AA23" t="inlineStr"/>
       <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="n">
-        <v>10.3</v>
+        <v>0.119</v>
       </c>
       <c r="AD23" t="n">
-        <v>13.95</v>
+        <v>3.11</v>
       </c>
       <c r="AE23" t="n">
         <v>1</v>
@@ -2200,43 +1974,43 @@
       <c r="AH23" t="inlineStr"/>
       <c r="AI23" t="inlineStr"/>
       <c r="AJ23" s="2" t="n">
-        <v>44375.61458333334</v>
+        <v>43389.29166666666</v>
       </c>
       <c r="AK23" t="inlineStr"/>
       <c r="AL23" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01_F-264</t>
+          <t>PB_1_003_04P001442_F-337</t>
         </is>
       </c>
       <c r="AM23" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01_1</t>
+          <t>PB_1_003_04P001442_1</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01</t>
+          <t>PB_1_003_04P001442</t>
         </is>
       </c>
       <c r="B24" t="n">
         <v>3</v>
       </c>
       <c r="C24" t="n">
-        <v>104701.575</v>
+        <v>105401.924</v>
       </c>
       <c r="D24" t="n">
-        <v>528274.6429999999</v>
+        <v>528165.52</v>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="n">
-        <v>7.851</v>
+        <v>-0.74</v>
       </c>
       <c r="H24" t="inlineStr"/>
       <c r="I24" s="2" t="n">
-        <v>43468.29166666666</v>
+        <v>43388.29166666666</v>
       </c>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
@@ -2258,10 +2032,10 @@
       <c r="AA24" t="inlineStr"/>
       <c r="AB24" t="inlineStr"/>
       <c r="AC24" t="n">
-        <v>7.351</v>
+        <v>-0.1</v>
       </c>
       <c r="AD24" t="n">
-        <v>29.8</v>
+        <v>29.61</v>
       </c>
       <c r="AE24" t="n">
         <v>1</v>
@@ -2271,46 +2045,36 @@
       <c r="AH24" t="inlineStr"/>
       <c r="AI24" t="inlineStr"/>
       <c r="AJ24" s="2" t="n">
-        <v>43468.29166666666</v>
-      </c>
-      <c r="AK24" s="2" t="n">
-        <v>43501.46527777778</v>
-      </c>
+        <v>43388.29166666666</v>
+      </c>
+      <c r="AK24" t="inlineStr"/>
       <c r="AL24" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01_F-2</t>
+          <t>PB_1_003_04P001442_F-2</t>
         </is>
       </c>
       <c r="AM24" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01_3</t>
+          <t>PB_1_003_04P001442_3</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01</t>
+          <t>PB_1_003_04P001442</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>3</v>
-      </c>
-      <c r="C25" t="n">
-        <v>104701.575</v>
-      </c>
-      <c r="D25" t="n">
-        <v>528274.6429999999</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
-      <c r="G25" t="n">
-        <v>7.851</v>
-      </c>
+      <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
-      <c r="I25" s="2" t="n">
-        <v>43501.46527777778</v>
-      </c>
+      <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
@@ -2330,59 +2094,49 @@
       <c r="Z25" t="inlineStr"/>
       <c r="AA25" t="inlineStr"/>
       <c r="AB25" t="inlineStr"/>
-      <c r="AC25" t="n">
-        <v>7.351</v>
-      </c>
-      <c r="AD25" t="n">
-        <v>29.8</v>
-      </c>
-      <c r="AE25" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC25" t="inlineStr"/>
+      <c r="AD25" t="inlineStr"/>
+      <c r="AE25" t="inlineStr"/>
       <c r="AF25" t="inlineStr"/>
       <c r="AG25" t="inlineStr"/>
       <c r="AH25" t="inlineStr"/>
       <c r="AI25" t="inlineStr"/>
-      <c r="AJ25" s="2" t="n">
-        <v>43501.46527777778</v>
-      </c>
-      <c r="AK25" s="2" t="n">
-        <v>44074.48055555556</v>
-      </c>
+      <c r="AJ25" t="inlineStr"/>
+      <c r="AK25" t="inlineStr"/>
       <c r="AL25" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01_F-2</t>
+          <t>PB_1_003_04P001442_F-937</t>
         </is>
       </c>
       <c r="AM25" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01_3</t>
+          <t>PB_1_003_04P001442_2</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01</t>
+          <t>PB_1_004_04P001442-01</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>104701.575</v>
+        <v>104741.43</v>
       </c>
       <c r="D26" t="n">
-        <v>528274.6429999999</v>
+        <v>528280.213</v>
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="n">
-        <v>7.851</v>
+        <v>10.208</v>
       </c>
       <c r="H26" t="inlineStr"/>
       <c r="I26" s="2" t="n">
-        <v>44074.48055555556</v>
+        <v>43389.29166666666</v>
       </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
@@ -2404,10 +2158,10 @@
       <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="inlineStr"/>
       <c r="AC26" t="n">
-        <v>9</v>
+        <v>11.338</v>
       </c>
       <c r="AD26" t="n">
-        <v>31.449</v>
+        <v>13.39</v>
       </c>
       <c r="AE26" t="n">
         <v>1</v>
@@ -2417,45 +2171,43 @@
       <c r="AH26" t="inlineStr"/>
       <c r="AI26" t="inlineStr"/>
       <c r="AJ26" s="2" t="n">
-        <v>44074.48055555556</v>
-      </c>
-      <c r="AK26" s="2" t="n">
-        <v>44375.61041666667</v>
-      </c>
+        <v>43389.29166666666</v>
+      </c>
+      <c r="AK26" t="inlineStr"/>
       <c r="AL26" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01_F-2</t>
+          <t>PB_1_004_04P001442-01_F-204</t>
         </is>
       </c>
       <c r="AM26" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01_3</t>
+          <t>PB_1_004_04P001442-01_1</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01</t>
+          <t>PB_1_004_04P001442-01</t>
         </is>
       </c>
       <c r="B27" t="n">
         <v>3</v>
       </c>
       <c r="C27" t="n">
-        <v>104701.575</v>
+        <v>104741.437</v>
       </c>
       <c r="D27" t="n">
-        <v>528274.6429999999</v>
+        <v>528280.191</v>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="n">
-        <v>9.699999999999999</v>
+        <v>10.24</v>
       </c>
       <c r="H27" t="inlineStr"/>
       <c r="I27" s="2" t="n">
-        <v>44375.61041666667</v>
+        <v>43389.29166666666</v>
       </c>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
@@ -2477,10 +2229,10 @@
       <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="inlineStr"/>
       <c r="AC27" t="n">
-        <v>10.45</v>
+        <v>11.34</v>
       </c>
       <c r="AD27" t="n">
-        <v>32.899</v>
+        <v>33.3</v>
       </c>
       <c r="AE27" t="n">
         <v>1</v>
@@ -2490,44 +2242,36 @@
       <c r="AH27" t="inlineStr"/>
       <c r="AI27" t="inlineStr"/>
       <c r="AJ27" s="2" t="n">
-        <v>44375.61041666667</v>
+        <v>43389.29166666666</v>
       </c>
       <c r="AK27" t="inlineStr"/>
       <c r="AL27" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01_F-2</t>
+          <t>PB_1_004_04P001442-01_F-2</t>
         </is>
       </c>
       <c r="AM27" t="inlineStr">
         <is>
-          <t>PB_1_005_04P001442-01_3</t>
+          <t>PB_1_004_04P001442-01_3</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>PB_2_001_04P001442</t>
+          <t>PB_1_004_04P001442-01</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" t="n">
-        <v>105138.183</v>
-      </c>
-      <c r="D28" t="n">
-        <v>529244.291</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
-      <c r="G28" t="n">
-        <v>-1.383</v>
-      </c>
+      <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
-      <c r="I28" s="2" t="n">
-        <v>43390.29166666666</v>
-      </c>
+      <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
@@ -2547,57 +2291,49 @@
       <c r="Z28" t="inlineStr"/>
       <c r="AA28" t="inlineStr"/>
       <c r="AB28" t="inlineStr"/>
-      <c r="AC28" t="n">
-        <v>0.9370000000000001</v>
-      </c>
-      <c r="AD28" t="n">
-        <v>2.49</v>
-      </c>
-      <c r="AE28" t="n">
-        <v>0.9999999999999998</v>
-      </c>
+      <c r="AC28" t="inlineStr"/>
+      <c r="AD28" t="inlineStr"/>
+      <c r="AE28" t="inlineStr"/>
       <c r="AF28" t="inlineStr"/>
       <c r="AG28" t="inlineStr"/>
       <c r="AH28" t="inlineStr"/>
       <c r="AI28" t="inlineStr"/>
-      <c r="AJ28" s="2" t="n">
-        <v>43390.29166666666</v>
-      </c>
+      <c r="AJ28" t="inlineStr"/>
       <c r="AK28" t="inlineStr"/>
       <c r="AL28" t="inlineStr">
         <is>
-          <t>PB_2_001_04P001442_F-209</t>
+          <t>PB_1_004_04P001442-01_F-1</t>
         </is>
       </c>
       <c r="AM28" t="inlineStr">
         <is>
-          <t>PB_2_001_04P001442_1</t>
+          <t>PB_1_004_04P001442-01_2</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>PB_2_001_04P001442</t>
+          <t>PB_1_005_04P001442-01</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C29" t="n">
-        <v>105138.1</v>
+        <v>104701.644</v>
       </c>
       <c r="D29" t="n">
-        <v>529244.254</v>
+        <v>528274.721</v>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="n">
-        <v>-1.39</v>
+        <v>7.84</v>
       </c>
       <c r="H29" t="inlineStr"/>
       <c r="I29" s="2" t="n">
-        <v>43390.29166666666</v>
+        <v>43468.29166666666</v>
       </c>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
@@ -2619,10 +2355,10 @@
       <c r="AA29" t="inlineStr"/>
       <c r="AB29" t="inlineStr"/>
       <c r="AC29" t="n">
-        <v>0.73</v>
+        <v>7.35</v>
       </c>
       <c r="AD29" t="n">
-        <v>28.42</v>
+        <v>11</v>
       </c>
       <c r="AE29" t="n">
         <v>1</v>
@@ -2632,45 +2368,45 @@
       <c r="AH29" t="inlineStr"/>
       <c r="AI29" t="inlineStr"/>
       <c r="AJ29" s="2" t="n">
-        <v>43390.29166666666</v>
+        <v>43468.29166666666</v>
       </c>
       <c r="AK29" s="2" t="n">
-        <v>44075.62916666667</v>
+        <v>43501.46666666667</v>
       </c>
       <c r="AL29" t="inlineStr">
         <is>
-          <t>PB_2_001_04P001442_F-2</t>
+          <t>PB_1_005_04P001442-01_F-264</t>
         </is>
       </c>
       <c r="AM29" t="inlineStr">
         <is>
-          <t>PB_2_001_04P001442_3</t>
+          <t>PB_1_005_04P001442-01_1</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>PB_2_001_04P001442</t>
+          <t>PB_1_005_04P001442-01</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C30" t="n">
-        <v>105138.1</v>
+        <v>104701.644</v>
       </c>
       <c r="D30" t="n">
-        <v>529244.254</v>
+        <v>528274.721</v>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="n">
-        <v>-1.39</v>
+        <v>7.84</v>
       </c>
       <c r="H30" t="inlineStr"/>
       <c r="I30" s="2" t="n">
-        <v>44075.62916666667</v>
+        <v>43501.46666666667</v>
       </c>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
@@ -2692,10 +2428,10 @@
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="inlineStr"/>
       <c r="AC30" t="n">
-        <v>0.73</v>
+        <v>7.35</v>
       </c>
       <c r="AD30" t="n">
-        <v>29.9</v>
+        <v>11</v>
       </c>
       <c r="AE30" t="n">
         <v>1</v>
@@ -2705,44 +2441,36 @@
       <c r="AH30" t="inlineStr"/>
       <c r="AI30" t="inlineStr"/>
       <c r="AJ30" s="2" t="n">
-        <v>44075.62916666667</v>
+        <v>43501.46666666667</v>
       </c>
       <c r="AK30" t="inlineStr"/>
       <c r="AL30" t="inlineStr">
         <is>
-          <t>PB_2_001_04P001442_F-2</t>
+          <t>PB_1_005_04P001442-01_F-264</t>
         </is>
       </c>
       <c r="AM30" t="inlineStr">
         <is>
-          <t>PB_2_001_04P001442_3</t>
+          <t>PB_1_005_04P001442-01_1</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>PB_2_002_04P001442</t>
+          <t>PB_1_005_04P001442-01</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" t="n">
-        <v>105353.122</v>
-      </c>
-      <c r="D31" t="n">
-        <v>529060.968</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
-      <c r="G31" t="n">
-        <v>-1.106</v>
-      </c>
+      <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
-      <c r="I31" s="2" t="n">
-        <v>43390.29166666666</v>
-      </c>
+      <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
@@ -2762,58 +2490,42 @@
       <c r="Z31" t="inlineStr"/>
       <c r="AA31" t="inlineStr"/>
       <c r="AB31" t="inlineStr"/>
-      <c r="AC31" t="n">
-        <v>-0.286</v>
-      </c>
-      <c r="AD31" t="n">
-        <v>2.95</v>
-      </c>
-      <c r="AE31" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC31" t="inlineStr"/>
+      <c r="AD31" t="inlineStr"/>
+      <c r="AE31" t="inlineStr"/>
       <c r="AF31" t="inlineStr"/>
       <c r="AG31" t="inlineStr"/>
       <c r="AH31" t="inlineStr"/>
       <c r="AI31" t="inlineStr"/>
-      <c r="AJ31" s="2" t="n">
-        <v>43390.29166666666</v>
-      </c>
+      <c r="AJ31" t="inlineStr"/>
       <c r="AK31" t="inlineStr"/>
       <c r="AL31" t="inlineStr">
         <is>
-          <t>PB_2_002_04P001442_F-297</t>
+          <t>PB_1_005_04P001442-01_F-2</t>
         </is>
       </c>
       <c r="AM31" t="inlineStr">
         <is>
-          <t>PB_2_002_04P001442_1</t>
+          <t>PB_1_005_04P001442-01_3</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>PB_2_002_04P001442</t>
+          <t>PB_1_005_04P001442-01</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>3</v>
-      </c>
-      <c r="C32" t="n">
-        <v>105353.138</v>
-      </c>
-      <c r="D32" t="n">
-        <v>529060.951</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
-      <c r="G32" t="n">
-        <v>-1.026</v>
-      </c>
+      <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>
-      <c r="I32" s="2" t="n">
-        <v>43390.29166666666</v>
-      </c>
+      <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
@@ -2833,59 +2545,49 @@
       <c r="Z32" t="inlineStr"/>
       <c r="AA32" t="inlineStr"/>
       <c r="AB32" t="inlineStr"/>
-      <c r="AC32" t="n">
-        <v>-0.276</v>
-      </c>
-      <c r="AD32" t="n">
-        <v>24.7</v>
-      </c>
-      <c r="AE32" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC32" t="inlineStr"/>
+      <c r="AD32" t="inlineStr"/>
+      <c r="AE32" t="inlineStr"/>
       <c r="AF32" t="inlineStr"/>
       <c r="AG32" t="inlineStr"/>
       <c r="AH32" t="inlineStr"/>
       <c r="AI32" t="inlineStr"/>
-      <c r="AJ32" s="2" t="n">
-        <v>43390.29166666666</v>
-      </c>
-      <c r="AK32" s="2" t="n">
-        <v>44076.25763888889</v>
-      </c>
+      <c r="AJ32" t="inlineStr"/>
+      <c r="AK32" t="inlineStr"/>
       <c r="AL32" t="inlineStr">
         <is>
-          <t>PB_2_002_04P001442_F-2</t>
+          <t>PB_1_005_04P001442-01_F-964</t>
         </is>
       </c>
       <c r="AM32" t="inlineStr">
         <is>
-          <t>PB_2_002_04P001442_3</t>
+          <t>PB_1_005_04P001442-01_2</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>PB_2_002_04P001442</t>
+          <t>PB_2_001_04P001442</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C33" t="n">
-        <v>105353.138</v>
+        <v>105138.183</v>
       </c>
       <c r="D33" t="n">
-        <v>529060.951</v>
+        <v>529244.291</v>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="n">
-        <v>-1.026</v>
+        <v>-1.383</v>
       </c>
       <c r="H33" t="inlineStr"/>
       <c r="I33" s="2" t="n">
-        <v>44076.25763888889</v>
+        <v>43390.29166666666</v>
       </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
@@ -2907,56 +2609,56 @@
       <c r="AA33" t="inlineStr"/>
       <c r="AB33" t="inlineStr"/>
       <c r="AC33" t="n">
-        <v>-0.276</v>
+        <v>0.9370000000000001</v>
       </c>
       <c r="AD33" t="n">
-        <v>26.9</v>
+        <v>2.49</v>
       </c>
       <c r="AE33" t="n">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AF33" t="inlineStr"/>
       <c r="AG33" t="inlineStr"/>
       <c r="AH33" t="inlineStr"/>
       <c r="AI33" t="inlineStr"/>
       <c r="AJ33" s="2" t="n">
-        <v>44076.25763888889</v>
+        <v>43390.29166666666</v>
       </c>
       <c r="AK33" t="inlineStr"/>
       <c r="AL33" t="inlineStr">
         <is>
-          <t>PB_2_002_04P001442_F-2</t>
+          <t>PB_2_001_04P001442_F-209</t>
         </is>
       </c>
       <c r="AM33" t="inlineStr">
         <is>
-          <t>PB_2_002_04P001442_3</t>
+          <t>PB_2_001_04P001442_1</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>PB_2_003_04P001442-01</t>
+          <t>PB_2_001_04P001442</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C34" t="n">
-        <v>104924.599</v>
+        <v>105138.1</v>
       </c>
       <c r="D34" t="n">
-        <v>529294.469</v>
+        <v>529244.254</v>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="n">
-        <v>1.993</v>
+        <v>-1.39</v>
       </c>
       <c r="H34" t="inlineStr"/>
       <c r="I34" s="2" t="n">
-        <v>43389.29166666666</v>
+        <v>43390.29166666666</v>
       </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr"/>
@@ -2978,10 +2680,10 @@
       <c r="AA34" t="inlineStr"/>
       <c r="AB34" t="inlineStr"/>
       <c r="AC34" t="n">
-        <v>2.753</v>
+        <v>0.73</v>
       </c>
       <c r="AD34" t="n">
-        <v>4.859999999999999</v>
+        <v>28.42</v>
       </c>
       <c r="AE34" t="n">
         <v>1</v>
@@ -2991,44 +2693,36 @@
       <c r="AH34" t="inlineStr"/>
       <c r="AI34" t="inlineStr"/>
       <c r="AJ34" s="2" t="n">
-        <v>43389.29166666666</v>
+        <v>43390.29166666666</v>
       </c>
       <c r="AK34" t="inlineStr"/>
       <c r="AL34" t="inlineStr">
         <is>
-          <t>PB_2_003_04P001442-01_F-206</t>
+          <t>PB_2_001_04P001442_F-2</t>
         </is>
       </c>
       <c r="AM34" t="inlineStr">
         <is>
-          <t>PB_2_003_04P001442-01_1</t>
+          <t>PB_2_001_04P001442_3</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>PB_2_003_04P001442-01</t>
+          <t>PB_2_001_04P001442</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>3</v>
-      </c>
-      <c r="C35" t="n">
-        <v>104924.593</v>
-      </c>
-      <c r="D35" t="n">
-        <v>529294.545</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
-      <c r="G35" t="n">
-        <v>1.96</v>
-      </c>
+      <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr"/>
-      <c r="I35" s="2" t="n">
-        <v>44074.37222222222</v>
-      </c>
+      <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
@@ -3048,57 +2742,49 @@
       <c r="Z35" t="inlineStr"/>
       <c r="AA35" t="inlineStr"/>
       <c r="AB35" t="inlineStr"/>
-      <c r="AC35" t="n">
-        <v>2.69</v>
-      </c>
-      <c r="AD35" t="n">
-        <v>26.2</v>
-      </c>
-      <c r="AE35" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC35" t="inlineStr"/>
+      <c r="AD35" t="inlineStr"/>
+      <c r="AE35" t="inlineStr"/>
       <c r="AF35" t="inlineStr"/>
       <c r="AG35" t="inlineStr"/>
       <c r="AH35" t="inlineStr"/>
       <c r="AI35" t="inlineStr"/>
-      <c r="AJ35" s="2" t="n">
-        <v>44074.37222222222</v>
-      </c>
+      <c r="AJ35" t="inlineStr"/>
       <c r="AK35" t="inlineStr"/>
       <c r="AL35" t="inlineStr">
         <is>
-          <t>PB_2_003_04P001442-01_F-2</t>
+          <t>PB_2_001_04P001442_F-889</t>
         </is>
       </c>
       <c r="AM35" t="inlineStr">
         <is>
-          <t>PB_2_003_04P001442-01_3</t>
+          <t>PB_2_001_04P001442_2</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>PB_2_003_04P001442-01</t>
+          <t>PB_2_002_04P001442</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C36" t="n">
-        <v>104924.593</v>
+        <v>105353.122</v>
       </c>
       <c r="D36" t="n">
-        <v>529294.545</v>
+        <v>529060.968</v>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="n">
-        <v>1.96</v>
+        <v>-1.106</v>
       </c>
       <c r="H36" t="inlineStr"/>
       <c r="I36" s="2" t="n">
-        <v>43389.29166666666</v>
+        <v>43390.29166666666</v>
       </c>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
@@ -3120,10 +2806,10 @@
       <c r="AA36" t="inlineStr"/>
       <c r="AB36" t="inlineStr"/>
       <c r="AC36" t="n">
-        <v>2.69</v>
+        <v>-0.286</v>
       </c>
       <c r="AD36" t="n">
-        <v>26.22</v>
+        <v>2.95</v>
       </c>
       <c r="AE36" t="n">
         <v>1</v>
@@ -3133,45 +2819,43 @@
       <c r="AH36" t="inlineStr"/>
       <c r="AI36" t="inlineStr"/>
       <c r="AJ36" s="2" t="n">
-        <v>43389.29166666666</v>
-      </c>
-      <c r="AK36" s="2" t="n">
-        <v>43474.43402777778</v>
-      </c>
+        <v>43390.29166666666</v>
+      </c>
+      <c r="AK36" t="inlineStr"/>
       <c r="AL36" t="inlineStr">
         <is>
-          <t>PB_2_003_04P001442-01_F-2</t>
+          <t>PB_2_002_04P001442_F-297</t>
         </is>
       </c>
       <c r="AM36" t="inlineStr">
         <is>
-          <t>PB_2_003_04P001442-01_3</t>
+          <t>PB_2_002_04P001442_1</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>PB_2_003_04P001442-01</t>
+          <t>PB_2_002_04P001442</t>
         </is>
       </c>
       <c r="B37" t="n">
         <v>3</v>
       </c>
       <c r="C37" t="n">
-        <v>104924.593</v>
+        <v>105353.138</v>
       </c>
       <c r="D37" t="n">
-        <v>529294.545</v>
+        <v>529060.951</v>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="n">
-        <v>1.96</v>
+        <v>-1.026</v>
       </c>
       <c r="H37" t="inlineStr"/>
       <c r="I37" s="2" t="n">
-        <v>43474.43402777778</v>
+        <v>43390.29166666666</v>
       </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
@@ -3193,10 +2877,10 @@
       <c r="AA37" t="inlineStr"/>
       <c r="AB37" t="inlineStr"/>
       <c r="AC37" t="n">
-        <v>2.69</v>
+        <v>-0.276</v>
       </c>
       <c r="AD37" t="n">
-        <v>26.22</v>
+        <v>24.7</v>
       </c>
       <c r="AE37" t="n">
         <v>1</v>
@@ -3206,46 +2890,36 @@
       <c r="AH37" t="inlineStr"/>
       <c r="AI37" t="inlineStr"/>
       <c r="AJ37" s="2" t="n">
-        <v>43474.43402777778</v>
-      </c>
-      <c r="AK37" s="2" t="n">
-        <v>44074.37222222222</v>
-      </c>
+        <v>43390.29166666666</v>
+      </c>
+      <c r="AK37" t="inlineStr"/>
       <c r="AL37" t="inlineStr">
         <is>
-          <t>PB_2_003_04P001442-01_F-2</t>
+          <t>PB_2_002_04P001442_F-2</t>
         </is>
       </c>
       <c r="AM37" t="inlineStr">
         <is>
-          <t>PB_2_003_04P001442-01_3</t>
+          <t>PB_2_002_04P001442_3</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>PB_6_001_04P001442-01</t>
+          <t>PB_2_002_04P001442</t>
         </is>
       </c>
       <c r="B38" t="n">
         <v>2</v>
       </c>
-      <c r="C38" t="n">
-        <v>105089.504</v>
-      </c>
-      <c r="D38" t="n">
-        <v>530028.407</v>
-      </c>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
-      <c r="G38" t="n">
-        <v>0.996</v>
-      </c>
+      <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr"/>
-      <c r="I38" s="2" t="n">
-        <v>43390.29166666666</v>
-      </c>
+      <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
@@ -3265,59 +2939,49 @@
       <c r="Z38" t="inlineStr"/>
       <c r="AA38" t="inlineStr"/>
       <c r="AB38" t="inlineStr"/>
-      <c r="AC38" t="n">
-        <v>2.496</v>
-      </c>
-      <c r="AD38" t="n">
-        <v>9.890000000000001</v>
-      </c>
-      <c r="AE38" t="n">
-        <v>1</v>
-      </c>
+      <c r="AC38" t="inlineStr"/>
+      <c r="AD38" t="inlineStr"/>
+      <c r="AE38" t="inlineStr"/>
       <c r="AF38" t="inlineStr"/>
       <c r="AG38" t="inlineStr"/>
       <c r="AH38" t="inlineStr"/>
       <c r="AI38" t="inlineStr"/>
-      <c r="AJ38" s="2" t="n">
-        <v>43390.29166666666</v>
-      </c>
-      <c r="AK38" s="2" t="n">
-        <v>44074.31805555556</v>
-      </c>
+      <c r="AJ38" t="inlineStr"/>
+      <c r="AK38" t="inlineStr"/>
       <c r="AL38" t="inlineStr">
         <is>
-          <t>PB_6_001_04P001442-01_F-875</t>
+          <t>PB_2_002_04P001442_F-897</t>
         </is>
       </c>
       <c r="AM38" t="inlineStr">
         <is>
-          <t>PB_6_001_04P001442-01_2</t>
+          <t>PB_2_002_04P001442_2</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>PB_6_001_04P001442-01</t>
+          <t>PB_2_003_04P001442-01</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" t="n">
-        <v>105089.504</v>
+        <v>104924.599</v>
       </c>
       <c r="D39" t="n">
-        <v>530028.407</v>
+        <v>529294.469</v>
       </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="n">
-        <v>0.996</v>
+        <v>1.993</v>
       </c>
       <c r="H39" t="inlineStr"/>
       <c r="I39" s="2" t="n">
-        <v>44074.31805555556</v>
+        <v>43389.29166666666</v>
       </c>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
@@ -3339,30 +3003,2230 @@
       <c r="AA39" t="inlineStr"/>
       <c r="AB39" t="inlineStr"/>
       <c r="AC39" t="n">
-        <v>2.496</v>
+        <v>2.753</v>
       </c>
       <c r="AD39" t="n">
-        <v>9.949999999999999</v>
+        <v>4.859999999999999</v>
       </c>
       <c r="AE39" t="n">
-        <v>1.000000000000001</v>
+        <v>1</v>
       </c>
       <c r="AF39" t="inlineStr"/>
       <c r="AG39" t="inlineStr"/>
       <c r="AH39" t="inlineStr"/>
       <c r="AI39" t="inlineStr"/>
       <c r="AJ39" s="2" t="n">
-        <v>44074.31805555556</v>
+        <v>43389.29166666666</v>
       </c>
       <c r="AK39" t="inlineStr"/>
       <c r="AL39" t="inlineStr">
         <is>
+          <t>PB_2_003_04P001442-01_F-206</t>
+        </is>
+      </c>
+      <c r="AM39" t="inlineStr">
+        <is>
+          <t>PB_2_003_04P001442-01_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>PB_2_003_04P001442-01</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>3</v>
+      </c>
+      <c r="C40" t="n">
+        <v>104924.593</v>
+      </c>
+      <c r="D40" t="n">
+        <v>529294.545</v>
+      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" s="2" t="n">
+        <v>43389.29166666666</v>
+      </c>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr"/>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr"/>
+      <c r="R40" t="inlineStr"/>
+      <c r="S40" t="inlineStr"/>
+      <c r="T40" t="inlineStr"/>
+      <c r="U40" t="inlineStr"/>
+      <c r="V40" t="inlineStr"/>
+      <c r="W40" t="inlineStr"/>
+      <c r="X40" t="inlineStr"/>
+      <c r="Y40" t="inlineStr"/>
+      <c r="Z40" t="inlineStr"/>
+      <c r="AA40" t="inlineStr"/>
+      <c r="AB40" t="inlineStr"/>
+      <c r="AC40" t="n">
+        <v>2.69</v>
+      </c>
+      <c r="AD40" t="n">
+        <v>26.22</v>
+      </c>
+      <c r="AE40" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF40" t="inlineStr"/>
+      <c r="AG40" t="inlineStr"/>
+      <c r="AH40" t="inlineStr"/>
+      <c r="AI40" t="inlineStr"/>
+      <c r="AJ40" s="2" t="n">
+        <v>43389.29166666666</v>
+      </c>
+      <c r="AK40" s="2" t="n">
+        <v>43474.43402777778</v>
+      </c>
+      <c r="AL40" t="inlineStr">
+        <is>
+          <t>PB_2_003_04P001442-01_F-2</t>
+        </is>
+      </c>
+      <c r="AM40" t="inlineStr">
+        <is>
+          <t>PB_2_003_04P001442-01_3</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>PB_2_003_04P001442-01</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>3</v>
+      </c>
+      <c r="C41" t="n">
+        <v>104924.593</v>
+      </c>
+      <c r="D41" t="n">
+        <v>529294.545</v>
+      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" s="2" t="n">
+        <v>43474.43402777778</v>
+      </c>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
+      <c r="Q41" t="inlineStr"/>
+      <c r="R41" t="inlineStr"/>
+      <c r="S41" t="inlineStr"/>
+      <c r="T41" t="inlineStr"/>
+      <c r="U41" t="inlineStr"/>
+      <c r="V41" t="inlineStr"/>
+      <c r="W41" t="inlineStr"/>
+      <c r="X41" t="inlineStr"/>
+      <c r="Y41" t="inlineStr"/>
+      <c r="Z41" t="inlineStr"/>
+      <c r="AA41" t="inlineStr"/>
+      <c r="AB41" t="inlineStr"/>
+      <c r="AC41" t="n">
+        <v>2.69</v>
+      </c>
+      <c r="AD41" t="n">
+        <v>26.22</v>
+      </c>
+      <c r="AE41" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF41" t="inlineStr"/>
+      <c r="AG41" t="inlineStr"/>
+      <c r="AH41" t="inlineStr"/>
+      <c r="AI41" t="inlineStr"/>
+      <c r="AJ41" s="2" t="n">
+        <v>43474.43402777778</v>
+      </c>
+      <c r="AK41" t="inlineStr"/>
+      <c r="AL41" t="inlineStr">
+        <is>
+          <t>PB_2_003_04P001442-01_F-2</t>
+        </is>
+      </c>
+      <c r="AM41" t="inlineStr">
+        <is>
+          <t>PB_2_003_04P001442-01_3</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>PB_2_003_04P001442-01</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr"/>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr"/>
+      <c r="R42" t="inlineStr"/>
+      <c r="S42" t="inlineStr"/>
+      <c r="T42" t="inlineStr"/>
+      <c r="U42" t="inlineStr"/>
+      <c r="V42" t="inlineStr"/>
+      <c r="W42" t="inlineStr"/>
+      <c r="X42" t="inlineStr"/>
+      <c r="Y42" t="inlineStr"/>
+      <c r="Z42" t="inlineStr"/>
+      <c r="AA42" t="inlineStr"/>
+      <c r="AB42" t="inlineStr"/>
+      <c r="AC42" t="inlineStr"/>
+      <c r="AD42" t="inlineStr"/>
+      <c r="AE42" t="inlineStr"/>
+      <c r="AF42" t="inlineStr"/>
+      <c r="AG42" t="inlineStr"/>
+      <c r="AH42" t="inlineStr"/>
+      <c r="AI42" t="inlineStr"/>
+      <c r="AJ42" t="inlineStr"/>
+      <c r="AK42" t="inlineStr"/>
+      <c r="AL42" t="inlineStr">
+        <is>
+          <t>PB_2_003_04P001442-01_F-906</t>
+        </is>
+      </c>
+      <c r="AM42" t="inlineStr">
+        <is>
+          <t>PB_2_003_04P001442-01_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>PB_3_001_04P001442_F</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>51</v>
+      </c>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr"/>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr"/>
+      <c r="R43" t="inlineStr"/>
+      <c r="S43" t="inlineStr"/>
+      <c r="T43" t="inlineStr"/>
+      <c r="U43" t="inlineStr"/>
+      <c r="V43" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
+      <c r="X43" t="inlineStr"/>
+      <c r="Y43" t="inlineStr"/>
+      <c r="Z43" t="inlineStr"/>
+      <c r="AA43" t="inlineStr"/>
+      <c r="AB43" t="inlineStr"/>
+      <c r="AC43" t="inlineStr"/>
+      <c r="AD43" t="inlineStr"/>
+      <c r="AE43" t="inlineStr"/>
+      <c r="AF43" t="inlineStr"/>
+      <c r="AG43" t="inlineStr"/>
+      <c r="AH43" t="inlineStr"/>
+      <c r="AI43" t="inlineStr"/>
+      <c r="AJ43" t="inlineStr"/>
+      <c r="AK43" t="inlineStr"/>
+      <c r="AL43" t="inlineStr">
+        <is>
+          <t>PB_3_001_04P001442_F</t>
+        </is>
+      </c>
+      <c r="AM43" t="inlineStr">
+        <is>
+          <t>PB_3_001_04P001442_F_51</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>PB_3_001_04P001442_F-2</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>661</v>
+      </c>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr"/>
+      <c r="R44" t="inlineStr"/>
+      <c r="S44" t="inlineStr"/>
+      <c r="T44" t="inlineStr"/>
+      <c r="U44" t="inlineStr"/>
+      <c r="V44" t="inlineStr"/>
+      <c r="W44" t="inlineStr"/>
+      <c r="X44" t="inlineStr"/>
+      <c r="Y44" t="inlineStr"/>
+      <c r="Z44" t="inlineStr"/>
+      <c r="AA44" t="inlineStr"/>
+      <c r="AB44" t="inlineStr"/>
+      <c r="AC44" t="inlineStr"/>
+      <c r="AD44" t="inlineStr"/>
+      <c r="AE44" t="inlineStr"/>
+      <c r="AF44" t="inlineStr"/>
+      <c r="AG44" t="inlineStr"/>
+      <c r="AH44" t="inlineStr"/>
+      <c r="AI44" t="inlineStr"/>
+      <c r="AJ44" t="inlineStr"/>
+      <c r="AK44" t="inlineStr"/>
+      <c r="AL44" t="inlineStr">
+        <is>
+          <t>PB_3_001_04P001442_F-2</t>
+        </is>
+      </c>
+      <c r="AM44" t="inlineStr">
+        <is>
+          <t>PB_3_001_04P001442_F-2_661</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>PB_3_001_04P001442_F-811</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
+      <c r="Q45" t="inlineStr"/>
+      <c r="R45" t="inlineStr"/>
+      <c r="S45" t="inlineStr"/>
+      <c r="T45" t="inlineStr"/>
+      <c r="U45" t="inlineStr"/>
+      <c r="V45" t="inlineStr"/>
+      <c r="W45" t="inlineStr"/>
+      <c r="X45" t="inlineStr"/>
+      <c r="Y45" t="inlineStr"/>
+      <c r="Z45" t="inlineStr"/>
+      <c r="AA45" t="inlineStr"/>
+      <c r="AB45" t="inlineStr"/>
+      <c r="AC45" t="inlineStr"/>
+      <c r="AD45" t="inlineStr"/>
+      <c r="AE45" t="inlineStr"/>
+      <c r="AF45" t="inlineStr"/>
+      <c r="AG45" t="inlineStr"/>
+      <c r="AH45" t="inlineStr"/>
+      <c r="AI45" t="inlineStr"/>
+      <c r="AJ45" t="inlineStr"/>
+      <c r="AK45" t="inlineStr"/>
+      <c r="AL45" t="inlineStr">
+        <is>
+          <t>PB_3_001_04P001442_F-811</t>
+        </is>
+      </c>
+      <c r="AM45" t="inlineStr">
+        <is>
+          <t>PB_3_001_04P001442_F-811_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>PB_4_001_04P001442_F</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>151</v>
+      </c>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr"/>
+      <c r="Q46" t="inlineStr"/>
+      <c r="R46" t="inlineStr"/>
+      <c r="S46" t="inlineStr"/>
+      <c r="T46" t="inlineStr"/>
+      <c r="U46" t="inlineStr"/>
+      <c r="V46" t="inlineStr"/>
+      <c r="W46" t="inlineStr"/>
+      <c r="X46" t="inlineStr"/>
+      <c r="Y46" t="inlineStr"/>
+      <c r="Z46" t="inlineStr"/>
+      <c r="AA46" t="inlineStr"/>
+      <c r="AB46" t="inlineStr"/>
+      <c r="AC46" t="inlineStr"/>
+      <c r="AD46" t="inlineStr"/>
+      <c r="AE46" t="inlineStr"/>
+      <c r="AF46" t="inlineStr"/>
+      <c r="AG46" t="inlineStr"/>
+      <c r="AH46" t="inlineStr"/>
+      <c r="AI46" t="inlineStr"/>
+      <c r="AJ46" t="inlineStr"/>
+      <c r="AK46" t="inlineStr"/>
+      <c r="AL46" t="inlineStr">
+        <is>
+          <t>PB_4_001_04P001442_F</t>
+        </is>
+      </c>
+      <c r="AM46" t="inlineStr">
+        <is>
+          <t>PB_4_001_04P001442_F_151</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>PB_4_002_04P001442_F</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>96</v>
+      </c>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr"/>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
+      <c r="Q47" t="inlineStr"/>
+      <c r="R47" t="inlineStr"/>
+      <c r="S47" t="inlineStr"/>
+      <c r="T47" t="inlineStr"/>
+      <c r="U47" t="inlineStr"/>
+      <c r="V47" t="inlineStr"/>
+      <c r="W47" t="inlineStr"/>
+      <c r="X47" t="inlineStr"/>
+      <c r="Y47" t="inlineStr"/>
+      <c r="Z47" t="inlineStr"/>
+      <c r="AA47" t="inlineStr"/>
+      <c r="AB47" t="inlineStr"/>
+      <c r="AC47" t="inlineStr"/>
+      <c r="AD47" t="inlineStr"/>
+      <c r="AE47" t="inlineStr"/>
+      <c r="AF47" t="inlineStr"/>
+      <c r="AG47" t="inlineStr"/>
+      <c r="AH47" t="inlineStr"/>
+      <c r="AI47" t="inlineStr"/>
+      <c r="AJ47" t="inlineStr"/>
+      <c r="AK47" t="inlineStr"/>
+      <c r="AL47" t="inlineStr">
+        <is>
+          <t>PB_4_002_04P001442_F</t>
+        </is>
+      </c>
+      <c r="AM47" t="inlineStr">
+        <is>
+          <t>PB_4_002_04P001442_F_96</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>PB_5_001_04P001442_F</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>159</v>
+      </c>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr"/>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr"/>
+      <c r="R48" t="inlineStr"/>
+      <c r="S48" t="inlineStr"/>
+      <c r="T48" t="inlineStr"/>
+      <c r="U48" t="inlineStr"/>
+      <c r="V48" t="inlineStr"/>
+      <c r="W48" t="inlineStr"/>
+      <c r="X48" t="inlineStr"/>
+      <c r="Y48" t="inlineStr"/>
+      <c r="Z48" t="inlineStr"/>
+      <c r="AA48" t="inlineStr"/>
+      <c r="AB48" t="inlineStr"/>
+      <c r="AC48" t="inlineStr"/>
+      <c r="AD48" t="inlineStr"/>
+      <c r="AE48" t="inlineStr"/>
+      <c r="AF48" t="inlineStr"/>
+      <c r="AG48" t="inlineStr"/>
+      <c r="AH48" t="inlineStr"/>
+      <c r="AI48" t="inlineStr"/>
+      <c r="AJ48" t="inlineStr"/>
+      <c r="AK48" t="inlineStr"/>
+      <c r="AL48" t="inlineStr">
+        <is>
+          <t>PB_5_001_04P001442_F</t>
+        </is>
+      </c>
+      <c r="AM48" t="inlineStr">
+        <is>
+          <t>PB_5_001_04P001442_F_159</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>PB_5_001_04P001442_F-909</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>1</v>
+      </c>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr"/>
+      <c r="Q49" t="inlineStr"/>
+      <c r="R49" t="inlineStr"/>
+      <c r="S49" t="inlineStr"/>
+      <c r="T49" t="inlineStr"/>
+      <c r="U49" t="inlineStr"/>
+      <c r="V49" t="inlineStr"/>
+      <c r="W49" t="inlineStr"/>
+      <c r="X49" t="inlineStr"/>
+      <c r="Y49" t="inlineStr"/>
+      <c r="Z49" t="inlineStr"/>
+      <c r="AA49" t="inlineStr"/>
+      <c r="AB49" t="inlineStr"/>
+      <c r="AC49" t="inlineStr"/>
+      <c r="AD49" t="inlineStr"/>
+      <c r="AE49" t="inlineStr"/>
+      <c r="AF49" t="inlineStr"/>
+      <c r="AG49" t="inlineStr"/>
+      <c r="AH49" t="inlineStr"/>
+      <c r="AI49" t="inlineStr"/>
+      <c r="AJ49" t="inlineStr"/>
+      <c r="AK49" t="inlineStr"/>
+      <c r="AL49" t="inlineStr">
+        <is>
+          <t>PB_5_001_04P001442_F-909</t>
+        </is>
+      </c>
+      <c r="AM49" t="inlineStr">
+        <is>
+          <t>PB_5_001_04P001442_F-909_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>PB_5_002_04P001442_F</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>187</v>
+      </c>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
+      <c r="Q50" t="inlineStr"/>
+      <c r="R50" t="inlineStr"/>
+      <c r="S50" t="inlineStr"/>
+      <c r="T50" t="inlineStr"/>
+      <c r="U50" t="inlineStr"/>
+      <c r="V50" t="inlineStr"/>
+      <c r="W50" t="inlineStr"/>
+      <c r="X50" t="inlineStr"/>
+      <c r="Y50" t="inlineStr"/>
+      <c r="Z50" t="inlineStr"/>
+      <c r="AA50" t="inlineStr"/>
+      <c r="AB50" t="inlineStr"/>
+      <c r="AC50" t="inlineStr"/>
+      <c r="AD50" t="inlineStr"/>
+      <c r="AE50" t="inlineStr"/>
+      <c r="AF50" t="inlineStr"/>
+      <c r="AG50" t="inlineStr"/>
+      <c r="AH50" t="inlineStr"/>
+      <c r="AI50" t="inlineStr"/>
+      <c r="AJ50" t="inlineStr"/>
+      <c r="AK50" t="inlineStr"/>
+      <c r="AL50" t="inlineStr">
+        <is>
+          <t>PB_5_002_04P001442_F</t>
+        </is>
+      </c>
+      <c r="AM50" t="inlineStr">
+        <is>
+          <t>PB_5_002_04P001442_F_187</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>PB_5_002_04P001442_F-1</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>87</v>
+      </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr"/>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
+      <c r="Q51" t="inlineStr"/>
+      <c r="R51" t="inlineStr"/>
+      <c r="S51" t="inlineStr"/>
+      <c r="T51" t="inlineStr"/>
+      <c r="U51" t="inlineStr"/>
+      <c r="V51" t="inlineStr"/>
+      <c r="W51" t="inlineStr"/>
+      <c r="X51" t="inlineStr"/>
+      <c r="Y51" t="inlineStr"/>
+      <c r="Z51" t="inlineStr"/>
+      <c r="AA51" t="inlineStr"/>
+      <c r="AB51" t="inlineStr"/>
+      <c r="AC51" t="inlineStr"/>
+      <c r="AD51" t="inlineStr"/>
+      <c r="AE51" t="inlineStr"/>
+      <c r="AF51" t="inlineStr"/>
+      <c r="AG51" t="inlineStr"/>
+      <c r="AH51" t="inlineStr"/>
+      <c r="AI51" t="inlineStr"/>
+      <c r="AJ51" t="inlineStr"/>
+      <c r="AK51" t="inlineStr"/>
+      <c r="AL51" t="inlineStr">
+        <is>
+          <t>PB_5_002_04P001442_F-1</t>
+        </is>
+      </c>
+      <c r="AM51" t="inlineStr">
+        <is>
+          <t>PB_5_002_04P001442_F-1_87</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>PB_6_001_04P001442-01</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>2</v>
+      </c>
+      <c r="C52" t="n">
+        <v>105089.504</v>
+      </c>
+      <c r="D52" t="n">
+        <v>530028.407</v>
+      </c>
+      <c r="E52" t="inlineStr"/>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="n">
+        <v>0.996</v>
+      </c>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" s="2" t="n">
+        <v>43390.29166666666</v>
+      </c>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
+      <c r="Q52" t="inlineStr"/>
+      <c r="R52" t="inlineStr"/>
+      <c r="S52" t="inlineStr"/>
+      <c r="T52" t="inlineStr"/>
+      <c r="U52" t="inlineStr"/>
+      <c r="V52" t="inlineStr"/>
+      <c r="W52" t="inlineStr"/>
+      <c r="X52" t="inlineStr"/>
+      <c r="Y52" t="inlineStr"/>
+      <c r="Z52" t="inlineStr"/>
+      <c r="AA52" t="inlineStr"/>
+      <c r="AB52" t="inlineStr"/>
+      <c r="AC52" t="n">
+        <v>2.496</v>
+      </c>
+      <c r="AD52" t="n">
+        <v>9.890000000000001</v>
+      </c>
+      <c r="AE52" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF52" t="inlineStr"/>
+      <c r="AG52" t="inlineStr"/>
+      <c r="AH52" t="inlineStr"/>
+      <c r="AI52" t="inlineStr"/>
+      <c r="AJ52" s="2" t="n">
+        <v>43390.29166666666</v>
+      </c>
+      <c r="AK52" t="inlineStr"/>
+      <c r="AL52" t="inlineStr">
+        <is>
           <t>PB_6_001_04P001442-01_F-875</t>
         </is>
       </c>
-      <c r="AM39" t="inlineStr">
+      <c r="AM52" t="inlineStr">
         <is>
           <t>PB_6_001_04P001442-01_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>PB_6_001_04P001442-01</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>3</v>
+      </c>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr"/>
+      <c r="R53" t="inlineStr"/>
+      <c r="S53" t="inlineStr"/>
+      <c r="T53" t="inlineStr"/>
+      <c r="U53" t="inlineStr"/>
+      <c r="V53" t="inlineStr"/>
+      <c r="W53" t="inlineStr"/>
+      <c r="X53" t="inlineStr"/>
+      <c r="Y53" t="inlineStr"/>
+      <c r="Z53" t="inlineStr"/>
+      <c r="AA53" t="inlineStr"/>
+      <c r="AB53" t="inlineStr"/>
+      <c r="AC53" t="inlineStr"/>
+      <c r="AD53" t="inlineStr"/>
+      <c r="AE53" t="inlineStr"/>
+      <c r="AF53" t="inlineStr"/>
+      <c r="AG53" t="inlineStr"/>
+      <c r="AH53" t="inlineStr"/>
+      <c r="AI53" t="inlineStr"/>
+      <c r="AJ53" t="inlineStr"/>
+      <c r="AK53" t="inlineStr"/>
+      <c r="AL53" t="inlineStr">
+        <is>
+          <t>PB_6_001_04P001442-01_F-2</t>
+        </is>
+      </c>
+      <c r="AM53" t="inlineStr">
+        <is>
+          <t>PB_6_001_04P001442-01_3</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>PB_6_001_04P001442-01</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>1</v>
+      </c>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
+      <c r="Q54" t="inlineStr"/>
+      <c r="R54" t="inlineStr"/>
+      <c r="S54" t="inlineStr"/>
+      <c r="T54" t="inlineStr"/>
+      <c r="U54" t="inlineStr"/>
+      <c r="V54" t="inlineStr"/>
+      <c r="W54" t="inlineStr"/>
+      <c r="X54" t="inlineStr"/>
+      <c r="Y54" t="inlineStr"/>
+      <c r="Z54" t="inlineStr"/>
+      <c r="AA54" t="inlineStr"/>
+      <c r="AB54" t="inlineStr"/>
+      <c r="AC54" t="inlineStr"/>
+      <c r="AD54" t="inlineStr"/>
+      <c r="AE54" t="inlineStr"/>
+      <c r="AF54" t="inlineStr"/>
+      <c r="AG54" t="inlineStr"/>
+      <c r="AH54" t="inlineStr"/>
+      <c r="AI54" t="inlineStr"/>
+      <c r="AJ54" t="inlineStr"/>
+      <c r="AK54" t="inlineStr"/>
+      <c r="AL54" t="inlineStr">
+        <is>
+          <t>PB_6_001_04P001442-01_F-245</t>
+        </is>
+      </c>
+      <c r="AM54" t="inlineStr">
+        <is>
+          <t>PB_6_001_04P001442-01_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>PB_ZSNH-1_T9421_F</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>50</v>
+      </c>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr"/>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr"/>
+      <c r="R55" t="inlineStr"/>
+      <c r="S55" t="inlineStr"/>
+      <c r="T55" t="inlineStr"/>
+      <c r="U55" t="inlineStr"/>
+      <c r="V55" t="inlineStr"/>
+      <c r="W55" t="inlineStr"/>
+      <c r="X55" t="inlineStr"/>
+      <c r="Y55" t="inlineStr"/>
+      <c r="Z55" t="inlineStr"/>
+      <c r="AA55" t="inlineStr"/>
+      <c r="AB55" t="inlineStr"/>
+      <c r="AC55" t="inlineStr"/>
+      <c r="AD55" t="inlineStr"/>
+      <c r="AE55" t="inlineStr"/>
+      <c r="AF55" t="inlineStr"/>
+      <c r="AG55" t="inlineStr"/>
+      <c r="AH55" t="inlineStr"/>
+      <c r="AI55" t="inlineStr"/>
+      <c r="AJ55" t="inlineStr"/>
+      <c r="AK55" t="inlineStr"/>
+      <c r="AL55" t="inlineStr">
+        <is>
+          <t>PB_ZSNH-1_T9421_F</t>
+        </is>
+      </c>
+      <c r="AM55" t="inlineStr">
+        <is>
+          <t>PB_ZSNH-1_T9421_F_50</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>ZSNH002_diep</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" t="n">
+        <v>105739</v>
+      </c>
+      <c r="D56" t="n">
+        <v>531576</v>
+      </c>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr"/>
+      <c r="R56" t="inlineStr"/>
+      <c r="S56" t="inlineStr"/>
+      <c r="T56" t="inlineStr"/>
+      <c r="U56" t="inlineStr"/>
+      <c r="V56" t="inlineStr"/>
+      <c r="W56" t="inlineStr"/>
+      <c r="X56" t="inlineStr"/>
+      <c r="Y56" t="inlineStr"/>
+      <c r="Z56" t="inlineStr"/>
+      <c r="AA56" t="inlineStr"/>
+      <c r="AB56" t="inlineStr"/>
+      <c r="AC56" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="AD56" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="AE56" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF56" t="inlineStr"/>
+      <c r="AG56" t="inlineStr"/>
+      <c r="AH56" t="inlineStr"/>
+      <c r="AI56" t="inlineStr"/>
+      <c r="AJ56" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK56" t="inlineStr"/>
+      <c r="AL56" t="inlineStr">
+        <is>
+          <t>ZSNH002_diep</t>
+        </is>
+      </c>
+      <c r="AM56" t="inlineStr">
+        <is>
+          <t>ZSNH002_diep_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>ZSNH002b</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>1</v>
+      </c>
+      <c r="C57" t="n">
+        <v>105732</v>
+      </c>
+      <c r="D57" t="n">
+        <v>531580</v>
+      </c>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="n">
+        <v>5.97</v>
+      </c>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr"/>
+      <c r="R57" t="inlineStr"/>
+      <c r="S57" t="inlineStr"/>
+      <c r="T57" t="inlineStr"/>
+      <c r="U57" t="inlineStr"/>
+      <c r="V57" t="inlineStr"/>
+      <c r="W57" t="inlineStr"/>
+      <c r="X57" t="inlineStr"/>
+      <c r="Y57" t="inlineStr"/>
+      <c r="Z57" t="inlineStr"/>
+      <c r="AA57" t="inlineStr"/>
+      <c r="AB57" t="inlineStr"/>
+      <c r="AC57" t="n">
+        <v>6.47</v>
+      </c>
+      <c r="AD57" t="n">
+        <v>6.97</v>
+      </c>
+      <c r="AE57" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF57" t="inlineStr"/>
+      <c r="AG57" t="inlineStr"/>
+      <c r="AH57" t="inlineStr"/>
+      <c r="AI57" t="inlineStr"/>
+      <c r="AJ57" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK57" t="inlineStr"/>
+      <c r="AL57" t="inlineStr">
+        <is>
+          <t>ZSNH002b</t>
+        </is>
+      </c>
+      <c r="AM57" t="inlineStr">
+        <is>
+          <t>ZSNH002b_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>ZSNH003</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" t="n">
+        <v>104679</v>
+      </c>
+      <c r="D58" t="n">
+        <v>526740</v>
+      </c>
+      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="n">
+        <v>6.94</v>
+      </c>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr"/>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
+      <c r="R58" t="inlineStr"/>
+      <c r="S58" t="inlineStr"/>
+      <c r="T58" t="inlineStr"/>
+      <c r="U58" t="inlineStr"/>
+      <c r="V58" t="inlineStr"/>
+      <c r="W58" t="inlineStr"/>
+      <c r="X58" t="inlineStr"/>
+      <c r="Y58" t="inlineStr"/>
+      <c r="Z58" t="inlineStr"/>
+      <c r="AA58" t="inlineStr"/>
+      <c r="AB58" t="inlineStr"/>
+      <c r="AC58" t="n">
+        <v>7.44</v>
+      </c>
+      <c r="AD58" t="n">
+        <v>7.94</v>
+      </c>
+      <c r="AE58" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF58" t="inlineStr"/>
+      <c r="AG58" t="inlineStr"/>
+      <c r="AH58" t="inlineStr"/>
+      <c r="AI58" t="inlineStr"/>
+      <c r="AJ58" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK58" t="inlineStr"/>
+      <c r="AL58" t="inlineStr">
+        <is>
+          <t>ZSNH003</t>
+        </is>
+      </c>
+      <c r="AM58" t="inlineStr">
+        <is>
+          <t>ZSNH003_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>ZSNH004a_diep</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" t="n">
+        <v>105229</v>
+      </c>
+      <c r="D59" t="n">
+        <v>529953</v>
+      </c>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="n">
+        <v>2.17</v>
+      </c>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr"/>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr"/>
+      <c r="R59" t="inlineStr"/>
+      <c r="S59" t="inlineStr"/>
+      <c r="T59" t="inlineStr"/>
+      <c r="U59" t="inlineStr"/>
+      <c r="V59" t="inlineStr"/>
+      <c r="W59" t="inlineStr"/>
+      <c r="X59" t="inlineStr"/>
+      <c r="Y59" t="inlineStr"/>
+      <c r="Z59" t="inlineStr"/>
+      <c r="AA59" t="inlineStr"/>
+      <c r="AB59" t="inlineStr"/>
+      <c r="AC59" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="AD59" t="n">
+        <v>16.17</v>
+      </c>
+      <c r="AE59" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF59" t="inlineStr"/>
+      <c r="AG59" t="inlineStr"/>
+      <c r="AH59" t="inlineStr"/>
+      <c r="AI59" t="inlineStr"/>
+      <c r="AJ59" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK59" t="inlineStr"/>
+      <c r="AL59" t="inlineStr">
+        <is>
+          <t>ZSNH004a_diep</t>
+        </is>
+      </c>
+      <c r="AM59" t="inlineStr">
+        <is>
+          <t>ZSNH004a_diep_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>ZSNH004a_ondiep</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" t="n">
+        <v>105229</v>
+      </c>
+      <c r="D60" t="n">
+        <v>529954</v>
+      </c>
+      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="inlineStr"/>
+      <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr"/>
+      <c r="Q60" t="inlineStr"/>
+      <c r="R60" t="inlineStr"/>
+      <c r="S60" t="inlineStr"/>
+      <c r="T60" t="inlineStr"/>
+      <c r="U60" t="inlineStr"/>
+      <c r="V60" t="inlineStr"/>
+      <c r="W60" t="inlineStr"/>
+      <c r="X60" t="inlineStr"/>
+      <c r="Y60" t="inlineStr"/>
+      <c r="Z60" t="inlineStr"/>
+      <c r="AA60" t="inlineStr"/>
+      <c r="AB60" t="inlineStr"/>
+      <c r="AC60" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="AD60" t="n">
+        <v>4.08</v>
+      </c>
+      <c r="AE60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF60" t="inlineStr"/>
+      <c r="AG60" t="inlineStr"/>
+      <c r="AH60" t="inlineStr"/>
+      <c r="AI60" t="inlineStr"/>
+      <c r="AJ60" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK60" t="inlineStr"/>
+      <c r="AL60" t="inlineStr">
+        <is>
+          <t>ZSNH004a_ondiep</t>
+        </is>
+      </c>
+      <c r="AM60" t="inlineStr">
+        <is>
+          <t>ZSNH004a_ondiep_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>ZSNH004c</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C61" t="n">
+        <v>105065</v>
+      </c>
+      <c r="D61" t="n">
+        <v>529987</v>
+      </c>
+      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
+      <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
+      <c r="N61" t="inlineStr"/>
+      <c r="O61" t="inlineStr"/>
+      <c r="P61" t="inlineStr"/>
+      <c r="Q61" t="inlineStr"/>
+      <c r="R61" t="inlineStr"/>
+      <c r="S61" t="inlineStr"/>
+      <c r="T61" t="inlineStr"/>
+      <c r="U61" t="inlineStr"/>
+      <c r="V61" t="inlineStr"/>
+      <c r="W61" t="inlineStr"/>
+      <c r="X61" t="inlineStr"/>
+      <c r="Y61" t="inlineStr"/>
+      <c r="Z61" t="inlineStr"/>
+      <c r="AA61" t="inlineStr"/>
+      <c r="AB61" t="inlineStr"/>
+      <c r="AC61" t="inlineStr"/>
+      <c r="AD61" t="inlineStr"/>
+      <c r="AE61" t="inlineStr"/>
+      <c r="AF61" t="inlineStr"/>
+      <c r="AG61" t="inlineStr"/>
+      <c r="AH61" t="inlineStr"/>
+      <c r="AI61" t="inlineStr"/>
+      <c r="AJ61" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK61" t="inlineStr"/>
+      <c r="AL61" t="inlineStr">
+        <is>
+          <t>ZSNH004c</t>
+        </is>
+      </c>
+      <c r="AM61" t="inlineStr">
+        <is>
+          <t>ZSNH004c_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>ZSNH004d</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>1</v>
+      </c>
+      <c r="C62" t="n">
+        <v>105219</v>
+      </c>
+      <c r="D62" t="n">
+        <v>529958</v>
+      </c>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr"/>
+      <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="inlineStr"/>
+      <c r="O62" t="inlineStr"/>
+      <c r="P62" t="inlineStr"/>
+      <c r="Q62" t="inlineStr"/>
+      <c r="R62" t="inlineStr"/>
+      <c r="S62" t="inlineStr"/>
+      <c r="T62" t="inlineStr"/>
+      <c r="U62" t="inlineStr"/>
+      <c r="V62" t="inlineStr"/>
+      <c r="W62" t="inlineStr"/>
+      <c r="X62" t="inlineStr"/>
+      <c r="Y62" t="inlineStr"/>
+      <c r="Z62" t="inlineStr"/>
+      <c r="AA62" t="inlineStr"/>
+      <c r="AB62" t="inlineStr"/>
+      <c r="AC62" t="n">
+        <v>5.72</v>
+      </c>
+      <c r="AD62" t="n">
+        <v>6.22</v>
+      </c>
+      <c r="AE62" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF62" t="inlineStr"/>
+      <c r="AG62" t="inlineStr"/>
+      <c r="AH62" t="inlineStr"/>
+      <c r="AI62" t="inlineStr"/>
+      <c r="AJ62" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK62" t="inlineStr"/>
+      <c r="AL62" t="inlineStr">
+        <is>
+          <t>ZSNH004d</t>
+        </is>
+      </c>
+      <c r="AM62" t="inlineStr">
+        <is>
+          <t>ZSNH004d_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>ZSNH005_diep</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" t="n">
+        <v>104663</v>
+      </c>
+      <c r="D63" t="n">
+        <v>527264</v>
+      </c>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="inlineStr"/>
+      <c r="O63" t="inlineStr"/>
+      <c r="P63" t="inlineStr"/>
+      <c r="Q63" t="inlineStr"/>
+      <c r="R63" t="inlineStr"/>
+      <c r="S63" t="inlineStr"/>
+      <c r="T63" t="inlineStr"/>
+      <c r="U63" t="inlineStr"/>
+      <c r="V63" t="inlineStr"/>
+      <c r="W63" t="inlineStr"/>
+      <c r="X63" t="inlineStr"/>
+      <c r="Y63" t="inlineStr"/>
+      <c r="Z63" t="inlineStr"/>
+      <c r="AA63" t="inlineStr"/>
+      <c r="AB63" t="inlineStr"/>
+      <c r="AC63" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="AD63" t="n">
+        <v>16.46</v>
+      </c>
+      <c r="AE63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF63" t="inlineStr"/>
+      <c r="AG63" t="inlineStr"/>
+      <c r="AH63" t="inlineStr"/>
+      <c r="AI63" t="inlineStr"/>
+      <c r="AJ63" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK63" t="inlineStr"/>
+      <c r="AL63" t="inlineStr">
+        <is>
+          <t>ZSNH005_diep</t>
+        </is>
+      </c>
+      <c r="AM63" t="inlineStr">
+        <is>
+          <t>ZSNH005_diep_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>ZSNH005b</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>1</v>
+      </c>
+      <c r="C64" t="n">
+        <v>104653</v>
+      </c>
+      <c r="D64" t="n">
+        <v>527266</v>
+      </c>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr"/>
+      <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr"/>
+      <c r="N64" t="inlineStr"/>
+      <c r="O64" t="inlineStr"/>
+      <c r="P64" t="inlineStr"/>
+      <c r="Q64" t="inlineStr"/>
+      <c r="R64" t="inlineStr"/>
+      <c r="S64" t="inlineStr"/>
+      <c r="T64" t="inlineStr"/>
+      <c r="U64" t="inlineStr"/>
+      <c r="V64" t="inlineStr"/>
+      <c r="W64" t="inlineStr"/>
+      <c r="X64" t="inlineStr"/>
+      <c r="Y64" t="inlineStr"/>
+      <c r="Z64" t="inlineStr"/>
+      <c r="AA64" t="inlineStr"/>
+      <c r="AB64" t="inlineStr"/>
+      <c r="AC64" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="AD64" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="AE64" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF64" t="inlineStr"/>
+      <c r="AG64" t="inlineStr"/>
+      <c r="AH64" t="inlineStr"/>
+      <c r="AI64" t="inlineStr"/>
+      <c r="AJ64" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK64" t="inlineStr"/>
+      <c r="AL64" t="inlineStr">
+        <is>
+          <t>ZSNH005b</t>
+        </is>
+      </c>
+      <c r="AM64" t="inlineStr">
+        <is>
+          <t>ZSNH005b_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>ZSNH006_diep</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>1</v>
+      </c>
+      <c r="C65" t="n">
+        <v>105449</v>
+      </c>
+      <c r="D65" t="n">
+        <v>530799</v>
+      </c>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="n">
+        <v>2.17</v>
+      </c>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
+      <c r="L65" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="inlineStr"/>
+      <c r="O65" t="inlineStr"/>
+      <c r="P65" t="inlineStr"/>
+      <c r="Q65" t="inlineStr"/>
+      <c r="R65" t="inlineStr"/>
+      <c r="S65" t="inlineStr"/>
+      <c r="T65" t="inlineStr"/>
+      <c r="U65" t="inlineStr"/>
+      <c r="V65" t="inlineStr"/>
+      <c r="W65" t="inlineStr"/>
+      <c r="X65" t="inlineStr"/>
+      <c r="Y65" t="inlineStr"/>
+      <c r="Z65" t="inlineStr"/>
+      <c r="AA65" t="inlineStr"/>
+      <c r="AB65" t="inlineStr"/>
+      <c r="AC65" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="AD65" t="n">
+        <v>15.17</v>
+      </c>
+      <c r="AE65" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF65" t="inlineStr"/>
+      <c r="AG65" t="inlineStr"/>
+      <c r="AH65" t="inlineStr"/>
+      <c r="AI65" t="inlineStr"/>
+      <c r="AJ65" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK65" t="inlineStr"/>
+      <c r="AL65" t="inlineStr">
+        <is>
+          <t>ZSNH006_diep</t>
+        </is>
+      </c>
+      <c r="AM65" t="inlineStr">
+        <is>
+          <t>ZSNH006_diep_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>ZSNH006_ondiep</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>1</v>
+      </c>
+      <c r="C66" t="n">
+        <v>105449</v>
+      </c>
+      <c r="D66" t="n">
+        <v>530798</v>
+      </c>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H66" t="inlineStr"/>
+      <c r="I66" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr"/>
+      <c r="L66" t="inlineStr"/>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="inlineStr"/>
+      <c r="O66" t="inlineStr"/>
+      <c r="P66" t="inlineStr"/>
+      <c r="Q66" t="inlineStr"/>
+      <c r="R66" t="inlineStr"/>
+      <c r="S66" t="inlineStr"/>
+      <c r="T66" t="inlineStr"/>
+      <c r="U66" t="inlineStr"/>
+      <c r="V66" t="inlineStr"/>
+      <c r="W66" t="inlineStr"/>
+      <c r="X66" t="inlineStr"/>
+      <c r="Y66" t="inlineStr"/>
+      <c r="Z66" t="inlineStr"/>
+      <c r="AA66" t="inlineStr"/>
+      <c r="AB66" t="inlineStr"/>
+      <c r="AC66" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="AD66" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="AE66" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF66" t="inlineStr"/>
+      <c r="AG66" t="inlineStr"/>
+      <c r="AH66" t="inlineStr"/>
+      <c r="AI66" t="inlineStr"/>
+      <c r="AJ66" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK66" t="inlineStr"/>
+      <c r="AL66" t="inlineStr">
+        <is>
+          <t>ZSNH006_ondiep</t>
+        </is>
+      </c>
+      <c r="AM66" t="inlineStr">
+        <is>
+          <t>ZSNH006_ondiep_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>ZSNH006b</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>1</v>
+      </c>
+      <c r="C67" t="n">
+        <v>105440</v>
+      </c>
+      <c r="D67" t="n">
+        <v>530802</v>
+      </c>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="H67" t="inlineStr"/>
+      <c r="I67" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr"/>
+      <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
+      <c r="N67" t="inlineStr"/>
+      <c r="O67" t="inlineStr"/>
+      <c r="P67" t="inlineStr"/>
+      <c r="Q67" t="inlineStr"/>
+      <c r="R67" t="inlineStr"/>
+      <c r="S67" t="inlineStr"/>
+      <c r="T67" t="inlineStr"/>
+      <c r="U67" t="inlineStr"/>
+      <c r="V67" t="inlineStr"/>
+      <c r="W67" t="inlineStr"/>
+      <c r="X67" t="inlineStr"/>
+      <c r="Y67" t="inlineStr"/>
+      <c r="Z67" t="inlineStr"/>
+      <c r="AA67" t="inlineStr"/>
+      <c r="AB67" t="inlineStr"/>
+      <c r="AC67" t="n">
+        <v>5.55</v>
+      </c>
+      <c r="AD67" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="AE67" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF67" t="inlineStr"/>
+      <c r="AG67" t="inlineStr"/>
+      <c r="AH67" t="inlineStr"/>
+      <c r="AI67" t="inlineStr"/>
+      <c r="AJ67" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK67" t="inlineStr"/>
+      <c r="AL67" t="inlineStr">
+        <is>
+          <t>ZSNH006b</t>
+        </is>
+      </c>
+      <c r="AM67" t="inlineStr">
+        <is>
+          <t>ZSNH006b_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>ZSNH007</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>1</v>
+      </c>
+      <c r="C68" t="n">
+        <v>105063</v>
+      </c>
+      <c r="D68" t="n">
+        <v>529270</v>
+      </c>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J68" t="inlineStr"/>
+      <c r="K68" t="inlineStr"/>
+      <c r="L68" t="inlineStr"/>
+      <c r="M68" t="inlineStr"/>
+      <c r="N68" t="inlineStr"/>
+      <c r="O68" t="inlineStr"/>
+      <c r="P68" t="inlineStr"/>
+      <c r="Q68" t="inlineStr"/>
+      <c r="R68" t="inlineStr"/>
+      <c r="S68" t="inlineStr"/>
+      <c r="T68" t="inlineStr"/>
+      <c r="U68" t="inlineStr"/>
+      <c r="V68" t="inlineStr"/>
+      <c r="W68" t="inlineStr"/>
+      <c r="X68" t="inlineStr"/>
+      <c r="Y68" t="inlineStr"/>
+      <c r="Z68" t="inlineStr"/>
+      <c r="AA68" t="inlineStr"/>
+      <c r="AB68" t="inlineStr"/>
+      <c r="AC68" t="n">
+        <v>5.72</v>
+      </c>
+      <c r="AD68" t="n">
+        <v>6.22</v>
+      </c>
+      <c r="AE68" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF68" t="inlineStr"/>
+      <c r="AG68" t="inlineStr"/>
+      <c r="AH68" t="inlineStr"/>
+      <c r="AI68" t="inlineStr"/>
+      <c r="AJ68" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK68" t="inlineStr"/>
+      <c r="AL68" t="inlineStr">
+        <is>
+          <t>ZSNH007</t>
+        </is>
+      </c>
+      <c r="AM68" t="inlineStr">
+        <is>
+          <t>ZSNH007_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>ZSNH008</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>1</v>
+      </c>
+      <c r="C69" t="n">
+        <v>104849</v>
+      </c>
+      <c r="D69" t="n">
+        <v>528225</v>
+      </c>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="H69" t="inlineStr"/>
+      <c r="I69" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J69" t="inlineStr"/>
+      <c r="K69" t="inlineStr"/>
+      <c r="L69" t="inlineStr"/>
+      <c r="M69" t="inlineStr"/>
+      <c r="N69" t="inlineStr"/>
+      <c r="O69" t="inlineStr"/>
+      <c r="P69" t="inlineStr"/>
+      <c r="Q69" t="inlineStr"/>
+      <c r="R69" t="inlineStr"/>
+      <c r="S69" t="inlineStr"/>
+      <c r="T69" t="inlineStr"/>
+      <c r="U69" t="inlineStr"/>
+      <c r="V69" t="inlineStr"/>
+      <c r="W69" t="inlineStr"/>
+      <c r="X69" t="inlineStr"/>
+      <c r="Y69" t="inlineStr"/>
+      <c r="Z69" t="inlineStr"/>
+      <c r="AA69" t="inlineStr"/>
+      <c r="AB69" t="inlineStr"/>
+      <c r="AC69" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="AD69" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="AE69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF69" t="inlineStr"/>
+      <c r="AG69" t="inlineStr"/>
+      <c r="AH69" t="inlineStr"/>
+      <c r="AI69" t="inlineStr"/>
+      <c r="AJ69" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK69" t="inlineStr"/>
+      <c r="AL69" t="inlineStr">
+        <is>
+          <t>ZSNH008</t>
+        </is>
+      </c>
+      <c r="AM69" t="inlineStr">
+        <is>
+          <t>ZSNH008_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>ZSNH009</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>1</v>
+      </c>
+      <c r="C70" t="n">
+        <v>104609</v>
+      </c>
+      <c r="D70" t="n">
+        <v>527055</v>
+      </c>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="n">
+        <v>5.59</v>
+      </c>
+      <c r="H70" t="inlineStr"/>
+      <c r="I70" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J70" t="inlineStr"/>
+      <c r="K70" t="inlineStr"/>
+      <c r="L70" t="inlineStr"/>
+      <c r="M70" t="inlineStr"/>
+      <c r="N70" t="inlineStr"/>
+      <c r="O70" t="inlineStr"/>
+      <c r="P70" t="inlineStr"/>
+      <c r="Q70" t="inlineStr"/>
+      <c r="R70" t="inlineStr"/>
+      <c r="S70" t="inlineStr"/>
+      <c r="T70" t="inlineStr"/>
+      <c r="U70" t="inlineStr"/>
+      <c r="V70" t="inlineStr"/>
+      <c r="W70" t="inlineStr"/>
+      <c r="X70" t="inlineStr"/>
+      <c r="Y70" t="inlineStr"/>
+      <c r="Z70" t="inlineStr"/>
+      <c r="AA70" t="inlineStr"/>
+      <c r="AB70" t="inlineStr"/>
+      <c r="AC70" t="n">
+        <v>6.09</v>
+      </c>
+      <c r="AD70" t="n">
+        <v>6.59</v>
+      </c>
+      <c r="AE70" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF70" t="inlineStr"/>
+      <c r="AG70" t="inlineStr"/>
+      <c r="AH70" t="inlineStr"/>
+      <c r="AI70" t="inlineStr"/>
+      <c r="AJ70" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK70" t="inlineStr"/>
+      <c r="AL70" t="inlineStr">
+        <is>
+          <t>ZSNH009</t>
+        </is>
+      </c>
+      <c r="AM70" t="inlineStr">
+        <is>
+          <t>ZSNH009_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>ZSNH010_diep</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>1</v>
+      </c>
+      <c r="C71" t="n">
+        <v>105543</v>
+      </c>
+      <c r="D71" t="n">
+        <v>531088</v>
+      </c>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="n">
+        <v>5.18</v>
+      </c>
+      <c r="H71" t="inlineStr"/>
+      <c r="I71" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J71" t="inlineStr"/>
+      <c r="K71" t="inlineStr"/>
+      <c r="L71" t="inlineStr"/>
+      <c r="M71" t="inlineStr"/>
+      <c r="N71" t="inlineStr"/>
+      <c r="O71" t="inlineStr"/>
+      <c r="P71" t="inlineStr"/>
+      <c r="Q71" t="inlineStr"/>
+      <c r="R71" t="inlineStr"/>
+      <c r="S71" t="inlineStr"/>
+      <c r="T71" t="inlineStr"/>
+      <c r="U71" t="inlineStr"/>
+      <c r="V71" t="inlineStr"/>
+      <c r="W71" t="inlineStr"/>
+      <c r="X71" t="inlineStr"/>
+      <c r="Y71" t="inlineStr"/>
+      <c r="Z71" t="inlineStr"/>
+      <c r="AA71" t="inlineStr"/>
+      <c r="AB71" t="inlineStr"/>
+      <c r="AC71" t="n">
+        <v>5.68</v>
+      </c>
+      <c r="AD71" t="n">
+        <v>15.18</v>
+      </c>
+      <c r="AE71" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF71" t="inlineStr"/>
+      <c r="AG71" t="inlineStr"/>
+      <c r="AH71" t="inlineStr"/>
+      <c r="AI71" t="inlineStr"/>
+      <c r="AJ71" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK71" t="inlineStr"/>
+      <c r="AL71" t="inlineStr">
+        <is>
+          <t>ZSNH010_diep</t>
+        </is>
+      </c>
+      <c r="AM71" t="inlineStr">
+        <is>
+          <t>ZSNH010_diep_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>ZSNH010b</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>1</v>
+      </c>
+      <c r="C72" t="n">
+        <v>105534</v>
+      </c>
+      <c r="D72" t="n">
+        <v>531090</v>
+      </c>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="H72" t="inlineStr"/>
+      <c r="I72" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J72" t="inlineStr"/>
+      <c r="K72" t="inlineStr"/>
+      <c r="L72" t="inlineStr"/>
+      <c r="M72" t="inlineStr"/>
+      <c r="N72" t="inlineStr"/>
+      <c r="O72" t="inlineStr"/>
+      <c r="P72" t="inlineStr"/>
+      <c r="Q72" t="inlineStr"/>
+      <c r="R72" t="inlineStr"/>
+      <c r="S72" t="inlineStr"/>
+      <c r="T72" t="inlineStr"/>
+      <c r="U72" t="inlineStr"/>
+      <c r="V72" t="inlineStr"/>
+      <c r="W72" t="inlineStr"/>
+      <c r="X72" t="inlineStr"/>
+      <c r="Y72" t="inlineStr"/>
+      <c r="Z72" t="inlineStr"/>
+      <c r="AA72" t="inlineStr"/>
+      <c r="AB72" t="inlineStr"/>
+      <c r="AC72" t="n">
+        <v>5.64</v>
+      </c>
+      <c r="AD72" t="n">
+        <v>6.14</v>
+      </c>
+      <c r="AE72" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF72" t="inlineStr"/>
+      <c r="AG72" t="inlineStr"/>
+      <c r="AH72" t="inlineStr"/>
+      <c r="AI72" t="inlineStr"/>
+      <c r="AJ72" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK72" t="inlineStr"/>
+      <c r="AL72" t="inlineStr">
+        <is>
+          <t>ZSNH010b</t>
+        </is>
+      </c>
+      <c r="AM72" t="inlineStr">
+        <is>
+          <t>ZSNH010b_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>ZSNH011b</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>1</v>
+      </c>
+      <c r="C73" t="n">
+        <v>105610</v>
+      </c>
+      <c r="D73" t="n">
+        <v>531327</v>
+      </c>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="H73" t="inlineStr"/>
+      <c r="I73" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="J73" t="inlineStr"/>
+      <c r="K73" t="inlineStr"/>
+      <c r="L73" t="inlineStr"/>
+      <c r="M73" t="inlineStr"/>
+      <c r="N73" t="inlineStr"/>
+      <c r="O73" t="inlineStr"/>
+      <c r="P73" t="inlineStr"/>
+      <c r="Q73" t="inlineStr"/>
+      <c r="R73" t="inlineStr"/>
+      <c r="S73" t="inlineStr"/>
+      <c r="T73" t="inlineStr"/>
+      <c r="U73" t="inlineStr"/>
+      <c r="V73" t="inlineStr"/>
+      <c r="W73" t="inlineStr"/>
+      <c r="X73" t="inlineStr"/>
+      <c r="Y73" t="inlineStr"/>
+      <c r="Z73" t="inlineStr"/>
+      <c r="AA73" t="inlineStr"/>
+      <c r="AB73" t="inlineStr"/>
+      <c r="AC73" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="AD73" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="AE73" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF73" t="inlineStr"/>
+      <c r="AG73" t="inlineStr"/>
+      <c r="AH73" t="inlineStr"/>
+      <c r="AI73" t="inlineStr"/>
+      <c r="AJ73" s="2" t="n">
+        <v>36526</v>
+      </c>
+      <c r="AK73" t="inlineStr"/>
+      <c r="AL73" t="inlineStr">
+        <is>
+          <t>ZSNH011b</t>
+        </is>
+      </c>
+      <c r="AM73" t="inlineStr">
+        <is>
+          <t>ZSNH011b_1</t>
         </is>
       </c>
     </row>

</xml_diff>